<commit_message>
Move U48 and update SHACL
</commit_message>
<xml_diff>
--- a/04-SHACL/philharmonie-chatbot-0.1-shacl.xlsx
+++ b/04-SHACL/philharmonie-chatbot-0.1-shacl.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="391">
   <si>
     <t xml:space="preserve">PREFIX</t>
   </si>
@@ -199,7 +199,7 @@
     <t xml:space="preserve">sh:IRI</t>
   </si>
   <si>
-    <t xml:space="preserve">^https://ark.philharmoniedeparis.fr/ark/49250/[0-9]*?$</t>
+    <t xml:space="preserve">^https://ark.philharmoniedeparis.fr/ark:49250/[0-9]*?$</t>
   </si>
   <si>
     <t xml:space="preserve">true</t>
@@ -211,7 +211,7 @@
     <t xml:space="preserve">efrbroo:F30_Publication_Event</t>
   </si>
   <si>
-    <t xml:space="preserve">^https://ark.philharmoniedeparis.fr/ark/49250/[0-9]*#event</t>
+    <t xml:space="preserve">^https://ark.philharmoniedeparis.fr/ark:49250/[0-9]*#event</t>
   </si>
   <si>
     <t xml:space="preserve">ecrm:E7_Activity</t>
@@ -430,6 +430,9 @@
     <t xml:space="preserve">mus:U168_has_parallel_title</t>
   </si>
   <si>
+    <t xml:space="preserve">0..n</t>
+  </si>
+  <si>
     <t xml:space="preserve">U168 has parallel title</t>
   </si>
   <si>
@@ -460,9 +463,6 @@
     <t xml:space="preserve">mus:U65_has_geographical_context</t>
   </si>
   <si>
-    <t xml:space="preserve">0..n</t>
-  </si>
-  <si>
     <t xml:space="preserve">U65 has geographical context</t>
   </si>
   <si>
@@ -514,6 +514,9 @@
     <t xml:space="preserve">Properties on mus:M167_Publication_Expression_Fragment</t>
   </si>
   <si>
+    <t xml:space="preserve">1..n</t>
+  </si>
+  <si>
     <t xml:space="preserve">Properties on efrbroo:F30_Publication_Event</t>
   </si>
   <si>
@@ -569,9 +572,6 @@
   </si>
   <si>
     <t xml:space="preserve">mus:U23_has_casting_detail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1..n</t>
   </si>
   <si>
     <t xml:space="preserve">M23 Casting Detail</t>
@@ -1211,7 +1211,7 @@
     <numFmt numFmtId="166" formatCode="General"/>
     <numFmt numFmtId="167" formatCode="0.00"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1346,11 +1346,6 @@
       <name val="Cambria"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -1793,7 +1788,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="84">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2026,10 +2021,6 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2062,14 +2053,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2095,18 +2086,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2134,7 +2117,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="26" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="26" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2285,10 +2268,10 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="1" sqref="D35 B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6953125" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.09"/>
   </cols>
@@ -2411,21 +2394,21 @@
   <dimension ref="A1:O1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="G12" activeCellId="1" sqref="D35 G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.54"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="3" min="3" style="4" width="27.86"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="4" min="4" style="0" width="42.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.45"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="4" min="4" style="0" width="42.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="57.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="28.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="5" width="24.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="25.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="25.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="4" width="23.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="68.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.54"/>
@@ -2947,18 +2930,18 @@
   <dimension ref="A1:AMJ76"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="7" topLeftCell="D53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="7" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
-      <selection pane="bottomRight" activeCell="D60" activeCellId="0" sqref="D60"/>
+      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="D35" activeCellId="0" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="34.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="40.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="24" width="36.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="29" width="37.79"/>
@@ -2967,19 +2950,18 @@
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="9" min="9" style="12" width="41.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="30" width="14.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="31" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="20.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="36.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="20.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="36.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="5" width="28.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="28.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="18" style="0" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="26.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="34.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="4" width="28.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="22.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="18.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="17" style="0" width="26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="26.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="34.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="4" width="28.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="22.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2991,7 +2973,7 @@
       </c>
       <c r="C1" s="2"/>
       <c r="F1" s="0"/>
-      <c r="U1" s="4"/>
+      <c r="T1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6"/>
@@ -3019,15 +3001,14 @@
       <c r="R3" s="8"/>
       <c r="S3" s="8"/>
       <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
+      <c r="U3" s="11"/>
       <c r="V3" s="11"/>
       <c r="W3" s="11"/>
-      <c r="X3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F4" s="36"/>
       <c r="J4" s="37"/>
-      <c r="V4" s="4"/>
+      <c r="U4" s="4"/>
     </row>
     <row r="5" s="15" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
@@ -3065,30 +3046,31 @@
       <c r="O5" s="16" t="s">
         <v>86</v>
       </c>
+      <c r="P5" s="15" t="s">
+        <v>87</v>
+      </c>
       <c r="Q5" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="R5" s="15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="S5" s="15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="T5" s="15" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="U5" s="15" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="V5" s="15" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="W5" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="X5" s="15" t="s">
         <v>94</v>
       </c>
+      <c r="AMI5" s="0"/>
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" s="41" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3120,6 +3102,7 @@
         <v>103</v>
       </c>
       <c r="O6" s="44"/>
+      <c r="AMI6" s="0"/>
       <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3169,33 +3152,30 @@
         <v>115</v>
       </c>
       <c r="P7" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q7" s="17" t="s">
         <v>114</v>
       </c>
+      <c r="Q7" s="46" t="s">
+        <v>116</v>
+      </c>
       <c r="R7" s="46" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="S7" s="46" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="T7" s="46" t="s">
-        <v>118</v>
-      </c>
-      <c r="U7" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="V7" s="17" t="s">
+      <c r="U7" s="17" t="s">
         <v>46</v>
       </c>
+      <c r="V7" s="46" t="s">
+        <v>120</v>
+      </c>
       <c r="W7" s="46" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="X7" s="46" t="s">
-        <v>121</v>
-      </c>
-      <c r="Y7" s="46" t="s">
         <v>122</v>
       </c>
     </row>
@@ -3209,7 +3189,8 @@
       <c r="J8" s="54"/>
       <c r="K8" s="54"/>
       <c r="O8" s="53"/>
-      <c r="X8" s="55"/>
+      <c r="W8" s="55"/>
+      <c r="AMI8" s="0"/>
       <c r="AMJ8" s="0"/>
     </row>
     <row r="9" s="57" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3220,43 +3201,44 @@
       <c r="B9" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="58" t="s">
+      <c r="C9" s="22" t="s">
         <v>124</v>
       </c>
       <c r="D9" s="57" t="s">
         <v>125</v>
       </c>
       <c r="E9" s="24"/>
-      <c r="F9" s="59" t="s">
+      <c r="F9" s="58" t="s">
         <v>126</v>
       </c>
-      <c r="G9" s="59"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="61" t="str">
+      <c r="G9" s="58"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="60" t="str">
         <f aca="false">IF(LEFT($D9,SEARCH("..",$D9,1)-1)="n","",IF(LEFT($D9,SEARCH("..",$D9,1)-1)="0","",LEFT($D9,SEARCH("..",$D9,1)-1)))</f>
         <v/>
       </c>
-      <c r="K9" s="61" t="str">
+      <c r="K9" s="60" t="str">
         <f aca="false">IF(RIGHT($D9,SEARCH("..",$D9,1)-1)="n","",IF(RIGHT($D9,SEARCH("..",$D9,1)-1)="0","",RIGHT($D9,SEARCH("..",$D9,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="L9" s="62" t="str">
+      <c r="L9" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E9,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M9" s="62" t="str">
+      <c r="M9" s="61" t="str">
         <f aca="false">IF(L9="sh:Literal",E9,"")</f>
         <v/>
       </c>
-      <c r="N9" s="62" t="str">
+      <c r="N9" s="61" t="str">
         <f aca="false">IF($L9="sh:IRI",IF($E9&lt;&gt;"",$E9,""),"")</f>
         <v/>
       </c>
-      <c r="O9" s="63" t="str">
+      <c r="O9" s="62" t="str">
         <f aca="false">IF($L9&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E9)-1,0)=0,"","1"))</f>
         <v/>
       </c>
-      <c r="W9" s="64"/>
+      <c r="V9" s="63"/>
+      <c r="AMI9" s="0"/>
       <c r="AMJ9" s="0"/>
     </row>
     <row r="10" s="57" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3273,38 +3255,39 @@
       <c r="D10" s="57" t="s">
         <v>125</v>
       </c>
-      <c r="E10" s="60"/>
-      <c r="F10" s="59" t="s">
+      <c r="E10" s="59"/>
+      <c r="F10" s="58" t="s">
         <v>128</v>
       </c>
-      <c r="G10" s="64"/>
-      <c r="H10" s="64"/>
-      <c r="I10" s="65"/>
-      <c r="J10" s="61" t="str">
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="64"/>
+      <c r="J10" s="60" t="str">
         <f aca="false">IF(LEFT($D10,SEARCH("..",$D10,1)-1)="n","",IF(LEFT($D10,SEARCH("..",$D10,1)-1)="0","",LEFT($D10,SEARCH("..",$D10,1)-1)))</f>
         <v/>
       </c>
-      <c r="K10" s="61" t="str">
+      <c r="K10" s="60" t="str">
         <f aca="false">IF(RIGHT($D10,SEARCH("..",$D10,1)-1)="n","",IF(RIGHT($D10,SEARCH("..",$D10,1)-1)="0","",RIGHT($D10,SEARCH("..",$D10,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="L10" s="62" t="str">
+      <c r="L10" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E10,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M10" s="62" t="str">
+      <c r="M10" s="61" t="str">
         <f aca="false">IF(L10="sh:Literal",E10,"")</f>
         <v/>
       </c>
-      <c r="N10" s="62" t="str">
+      <c r="N10" s="61" t="str">
         <f aca="false">IF($L10="sh:IRI",IF($E10&lt;&gt;"",$E10,""),"")</f>
         <v/>
       </c>
-      <c r="O10" s="63" t="str">
+      <c r="O10" s="62" t="str">
         <f aca="false">IF($L10&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E10)-1,0)=0,"","1"))</f>
         <v/>
       </c>
-      <c r="W10" s="64"/>
+      <c r="V10" s="63"/>
+      <c r="AMI10" s="0"/>
       <c r="AMJ10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3324,30 +3307,30 @@
       <c r="E11" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="F11" s="59" t="s">
+      <c r="F11" s="58" t="s">
         <v>130</v>
       </c>
-      <c r="J11" s="61" t="str">
+      <c r="J11" s="60" t="str">
         <f aca="false">IF(LEFT($D11,SEARCH("..",$D11,1)-1)="n","",IF(LEFT($D11,SEARCH("..",$D11,1)-1)="0","",LEFT($D11,SEARCH("..",$D11,1)-1)))</f>
         <v/>
       </c>
-      <c r="K11" s="61" t="str">
+      <c r="K11" s="60" t="str">
         <f aca="false">IF(RIGHT($D11,SEARCH("..",$D11,1)-1)="n","",IF(RIGHT($D11,SEARCH("..",$D11,1)-1)="0","",RIGHT($D11,SEARCH("..",$D11,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="L11" s="62" t="str">
+      <c r="L11" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E11,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M11" s="62" t="str">
+      <c r="M11" s="61" t="str">
         <f aca="false">IF(L11="sh:Literal",E11,"")</f>
         <v/>
       </c>
-      <c r="N11" s="62" t="str">
+      <c r="N11" s="61" t="str">
         <f aca="false">IF($L11="sh:IRI",IF($E11&lt;&gt;"",$E11,""),"")</f>
         <v>mus:M156_Title_Statement</v>
       </c>
-      <c r="O11" s="63" t="str">
+      <c r="O11" s="62" t="str">
         <f aca="false">IF($L11&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E11)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -3369,30 +3352,30 @@
       <c r="E12" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="F12" s="59" t="s">
+      <c r="F12" s="58" t="s">
         <v>132</v>
       </c>
-      <c r="J12" s="61" t="str">
+      <c r="J12" s="60" t="str">
         <f aca="false">IF(LEFT($D12,SEARCH("..",$D12,1)-1)="n","",IF(LEFT($D12,SEARCH("..",$D12,1)-1)="0","",LEFT($D12,SEARCH("..",$D12,1)-1)))</f>
         <v/>
       </c>
-      <c r="K12" s="61" t="str">
+      <c r="K12" s="60" t="str">
         <f aca="false">IF(RIGHT($D12,SEARCH("..",$D12,1)-1)="n","",IF(RIGHT($D12,SEARCH("..",$D12,1)-1)="0","",RIGHT($D12,SEARCH("..",$D12,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="L12" s="62" t="str">
+      <c r="L12" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E12,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M12" s="62" t="str">
+      <c r="M12" s="61" t="str">
         <f aca="false">IF(L12="sh:Literal",E12,"")</f>
         <v/>
       </c>
-      <c r="N12" s="62" t="str">
+      <c r="N12" s="61" t="str">
         <f aca="false">IF($L12="sh:IRI",IF($E12&lt;&gt;"",$E12,""),"")</f>
         <v>mus:M157_Statement_of_Responsibility</v>
       </c>
-      <c r="O12" s="63" t="str">
+      <c r="O12" s="62" t="str">
         <f aca="false">IF($L12&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E12)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -3409,35 +3392,35 @@
         <v>133</v>
       </c>
       <c r="D13" s="57" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="E13" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="59" t="s">
-        <v>134</v>
-      </c>
-      <c r="J13" s="61" t="str">
+      <c r="F13" s="58" t="s">
+        <v>135</v>
+      </c>
+      <c r="J13" s="60" t="str">
         <f aca="false">IF(LEFT($D13,SEARCH("..",$D13,1)-1)="n","",IF(LEFT($D13,SEARCH("..",$D13,1)-1)="0","",LEFT($D13,SEARCH("..",$D13,1)-1)))</f>
         <v/>
       </c>
-      <c r="K13" s="61" t="str">
+      <c r="K13" s="60" t="str">
         <f aca="false">IF(RIGHT($D13,SEARCH("..",$D13,1)-1)="n","",IF(RIGHT($D13,SEARCH("..",$D13,1)-1)="0","",RIGHT($D13,SEARCH("..",$D13,1)-1)))</f>
-        <v>1</v>
-      </c>
-      <c r="L13" s="62" t="str">
+        <v/>
+      </c>
+      <c r="L13" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E13,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M13" s="62" t="str">
+      <c r="M13" s="61" t="str">
         <f aca="false">IF(L13="sh:Literal",E13,"")</f>
         <v/>
       </c>
-      <c r="N13" s="62" t="str">
+      <c r="N13" s="61" t="str">
         <f aca="false">IF($L13="sh:IRI",IF($E13&lt;&gt;"",$E13,""),"")</f>
         <v>ecrm:E35_Title</v>
       </c>
-      <c r="O13" s="63" t="str">
+      <c r="O13" s="62" t="str">
         <f aca="false">IF($L13&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E13)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -3451,38 +3434,38 @@
         <v>54</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D14" s="57" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="E14" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="59" t="s">
-        <v>136</v>
-      </c>
-      <c r="J14" s="61" t="str">
+      <c r="F14" s="58" t="s">
+        <v>137</v>
+      </c>
+      <c r="J14" s="60" t="str">
         <f aca="false">IF(LEFT($D14,SEARCH("..",$D14,1)-1)="n","",IF(LEFT($D14,SEARCH("..",$D14,1)-1)="0","",LEFT($D14,SEARCH("..",$D14,1)-1)))</f>
         <v/>
       </c>
-      <c r="K14" s="61" t="str">
+      <c r="K14" s="60" t="str">
         <f aca="false">IF(RIGHT($D14,SEARCH("..",$D14,1)-1)="n","",IF(RIGHT($D14,SEARCH("..",$D14,1)-1)="0","",RIGHT($D14,SEARCH("..",$D14,1)-1)))</f>
-        <v>1</v>
-      </c>
-      <c r="L14" s="62" t="str">
+        <v/>
+      </c>
+      <c r="L14" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E14,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M14" s="62" t="str">
+      <c r="M14" s="61" t="str">
         <f aca="false">IF(L14="sh:Literal",E14,"")</f>
         <v/>
       </c>
-      <c r="N14" s="62" t="str">
+      <c r="N14" s="61" t="str">
         <f aca="false">IF($L14="sh:IRI",IF($E14&lt;&gt;"",$E14,""),"")</f>
         <v>ecrm:E35_Title</v>
       </c>
-      <c r="O14" s="63" t="str">
+      <c r="O14" s="62" t="str">
         <f aca="false">IF($L14&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E14)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -3496,38 +3479,38 @@
         <v>54</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D15" s="57" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="E15" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="F15" s="59" t="s">
-        <v>138</v>
-      </c>
-      <c r="J15" s="61" t="str">
+      <c r="F15" s="58" t="s">
+        <v>139</v>
+      </c>
+      <c r="J15" s="60" t="str">
         <f aca="false">IF(LEFT($D15,SEARCH("..",$D15,1)-1)="n","",IF(LEFT($D15,SEARCH("..",$D15,1)-1)="0","",LEFT($D15,SEARCH("..",$D15,1)-1)))</f>
         <v/>
       </c>
-      <c r="K15" s="61" t="str">
+      <c r="K15" s="60" t="str">
         <f aca="false">IF(RIGHT($D15,SEARCH("..",$D15,1)-1)="n","",IF(RIGHT($D15,SEARCH("..",$D15,1)-1)="0","",RIGHT($D15,SEARCH("..",$D15,1)-1)))</f>
-        <v>1</v>
-      </c>
-      <c r="L15" s="62" t="str">
+        <v/>
+      </c>
+      <c r="L15" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E15,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M15" s="62" t="str">
+      <c r="M15" s="61" t="str">
         <f aca="false">IF(L15="sh:Literal",E15,"")</f>
         <v/>
       </c>
-      <c r="N15" s="62" t="str">
+      <c r="N15" s="61" t="str">
         <f aca="false">IF($L15="sh:IRI",IF($E15&lt;&gt;"",$E15,""),"")</f>
         <v>mus:M159_Edition_Statement</v>
       </c>
-      <c r="O15" s="63" t="str">
+      <c r="O15" s="62" t="str">
         <f aca="false">IF($L15&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E15)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -3541,7 +3524,7 @@
         <v>54</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D16" s="57" t="s">
         <v>125</v>
@@ -3549,30 +3532,30 @@
       <c r="E16" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="F16" s="59" t="s">
-        <v>140</v>
-      </c>
-      <c r="J16" s="61" t="str">
+      <c r="F16" s="58" t="s">
+        <v>141</v>
+      </c>
+      <c r="J16" s="60" t="str">
         <f aca="false">IF(LEFT($D16,SEARCH("..",$D16,1)-1)="n","",IF(LEFT($D16,SEARCH("..",$D16,1)-1)="0","",LEFT($D16,SEARCH("..",$D16,1)-1)))</f>
         <v/>
       </c>
-      <c r="K16" s="61" t="str">
+      <c r="K16" s="60" t="str">
         <f aca="false">IF(RIGHT($D16,SEARCH("..",$D16,1)-1)="n","",IF(RIGHT($D16,SEARCH("..",$D16,1)-1)="0","",RIGHT($D16,SEARCH("..",$D16,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="L16" s="62" t="str">
+      <c r="L16" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E16,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M16" s="62" t="str">
+      <c r="M16" s="61" t="str">
         <f aca="false">IF(L16="sh:Literal",E16,"")</f>
         <v/>
       </c>
-      <c r="N16" s="62" t="str">
+      <c r="N16" s="61" t="str">
         <f aca="false">IF($L16="sh:IRI",IF($E16&lt;&gt;"",$E16,""),"")</f>
         <v>mus:M163_Music_Format_Statement</v>
       </c>
-      <c r="O16" s="63" t="str">
+      <c r="O16" s="62" t="str">
         <f aca="false">IF($L16&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E16)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -3586,38 +3569,38 @@
         <v>54</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D17" s="57" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="E17" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="F17" s="59" t="s">
-        <v>142</v>
-      </c>
-      <c r="J17" s="61" t="str">
+      <c r="F17" s="58" t="s">
+        <v>143</v>
+      </c>
+      <c r="J17" s="60" t="str">
         <f aca="false">IF(LEFT($D17,SEARCH("..",$D17,1)-1)="n","",IF(LEFT($D17,SEARCH("..",$D17,1)-1)="0","",LEFT($D17,SEARCH("..",$D17,1)-1)))</f>
         <v/>
       </c>
-      <c r="K17" s="61" t="str">
+      <c r="K17" s="60" t="str">
         <f aca="false">IF(RIGHT($D17,SEARCH("..",$D17,1)-1)="n","",IF(RIGHT($D17,SEARCH("..",$D17,1)-1)="0","",RIGHT($D17,SEARCH("..",$D17,1)-1)))</f>
-        <v>1</v>
-      </c>
-      <c r="L17" s="62" t="str">
+        <v/>
+      </c>
+      <c r="L17" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E17,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M17" s="62" t="str">
+      <c r="M17" s="61" t="str">
         <f aca="false">IF(L17="sh:Literal",E17,"")</f>
         <v/>
       </c>
-      <c r="N17" s="62" t="str">
+      <c r="N17" s="61" t="str">
         <f aca="false">IF($L17="sh:IRI",IF($E17&lt;&gt;"",$E17,""),"")</f>
         <v>mus:M160_Publication_Statement</v>
       </c>
-      <c r="O17" s="63" t="str">
+      <c r="O17" s="62" t="str">
         <f aca="false">IF($L17&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E17)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -3630,36 +3613,36 @@
       <c r="B18" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="58" t="s">
-        <v>143</v>
+      <c r="C18" s="22" t="s">
+        <v>144</v>
       </c>
       <c r="D18" s="57" t="s">
-        <v>144</v>
-      </c>
-      <c r="F18" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="F18" s="58" t="s">
         <v>145</v>
       </c>
-      <c r="J18" s="61" t="str">
+      <c r="J18" s="60" t="str">
         <f aca="false">IF(LEFT($D18,SEARCH("..",$D18,1)-1)="n","",IF(LEFT($D18,SEARCH("..",$D18,1)-1)="0","",LEFT($D18,SEARCH("..",$D18,1)-1)))</f>
         <v/>
       </c>
-      <c r="K18" s="61" t="str">
+      <c r="K18" s="60" t="str">
         <f aca="false">IF(RIGHT($D18,SEARCH("..",$D18,1)-1)="n","",IF(RIGHT($D18,SEARCH("..",$D18,1)-1)="0","",RIGHT($D18,SEARCH("..",$D18,1)-1)))</f>
         <v/>
       </c>
-      <c r="L18" s="62" t="str">
+      <c r="L18" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E18,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M18" s="62" t="str">
+      <c r="M18" s="61" t="str">
         <f aca="false">IF(L18="sh:Literal",E18,"")</f>
         <v/>
       </c>
-      <c r="N18" s="62" t="str">
+      <c r="N18" s="61" t="str">
         <f aca="false">IF($L18="sh:IRI",IF($E18&lt;&gt;"",$E18,""),"")</f>
         <v/>
       </c>
-      <c r="O18" s="63" t="str">
+      <c r="O18" s="62" t="str">
         <f aca="false">IF($L18&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E18)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -3672,36 +3655,36 @@
       <c r="B19" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="58" t="s">
+      <c r="C19" s="22" t="s">
         <v>146</v>
       </c>
       <c r="D19" s="57" t="s">
-        <v>144</v>
-      </c>
-      <c r="F19" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="F19" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="J19" s="61" t="str">
+      <c r="J19" s="60" t="str">
         <f aca="false">IF(LEFT($D19,SEARCH("..",$D19,1)-1)="n","",IF(LEFT($D19,SEARCH("..",$D19,1)-1)="0","",LEFT($D19,SEARCH("..",$D19,1)-1)))</f>
         <v/>
       </c>
-      <c r="K19" s="61" t="str">
+      <c r="K19" s="60" t="str">
         <f aca="false">IF(RIGHT($D19,SEARCH("..",$D19,1)-1)="n","",IF(RIGHT($D19,SEARCH("..",$D19,1)-1)="0","",RIGHT($D19,SEARCH("..",$D19,1)-1)))</f>
         <v/>
       </c>
-      <c r="L19" s="62" t="str">
+      <c r="L19" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E19,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M19" s="62" t="str">
+      <c r="M19" s="61" t="str">
         <f aca="false">IF(L19="sh:Literal",E19,"")</f>
         <v/>
       </c>
-      <c r="N19" s="62" t="str">
+      <c r="N19" s="61" t="str">
         <f aca="false">IF($L19="sh:IRI",IF($E19&lt;&gt;"",$E19,""),"")</f>
         <v/>
       </c>
-      <c r="O19" s="63" t="str">
+      <c r="O19" s="62" t="str">
         <f aca="false">IF($L19&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E19)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -3714,36 +3697,36 @@
       <c r="B20" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="58" t="s">
+      <c r="C20" s="22" t="s">
         <v>148</v>
       </c>
       <c r="D20" s="57" t="s">
-        <v>144</v>
-      </c>
-      <c r="F20" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="F20" s="58" t="s">
         <v>149</v>
       </c>
-      <c r="J20" s="61" t="str">
+      <c r="J20" s="60" t="str">
         <f aca="false">IF(LEFT($D20,SEARCH("..",$D20,1)-1)="n","",IF(LEFT($D20,SEARCH("..",$D20,1)-1)="0","",LEFT($D20,SEARCH("..",$D20,1)-1)))</f>
         <v/>
       </c>
-      <c r="K20" s="61" t="str">
+      <c r="K20" s="60" t="str">
         <f aca="false">IF(RIGHT($D20,SEARCH("..",$D20,1)-1)="n","",IF(RIGHT($D20,SEARCH("..",$D20,1)-1)="0","",RIGHT($D20,SEARCH("..",$D20,1)-1)))</f>
         <v/>
       </c>
-      <c r="L20" s="62" t="str">
+      <c r="L20" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E20,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M20" s="62" t="str">
+      <c r="M20" s="61" t="str">
         <f aca="false">IF(L20="sh:Literal",E20,"")</f>
         <v/>
       </c>
-      <c r="N20" s="62" t="str">
+      <c r="N20" s="61" t="str">
         <f aca="false">IF($L20="sh:IRI",IF($E20&lt;&gt;"",$E20,""),"")</f>
         <v/>
       </c>
-      <c r="O20" s="63" t="str">
+      <c r="O20" s="62" t="str">
         <f aca="false">IF($L20&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E20)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -3756,36 +3739,36 @@
       <c r="B21" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="58" t="s">
+      <c r="C21" s="22" t="s">
         <v>150</v>
       </c>
       <c r="D21" s="57" t="s">
-        <v>144</v>
-      </c>
-      <c r="F21" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="F21" s="58" t="s">
         <v>151</v>
       </c>
-      <c r="J21" s="61" t="str">
+      <c r="J21" s="60" t="str">
         <f aca="false">IF(LEFT($D21,SEARCH("..",$D21,1)-1)="n","",IF(LEFT($D21,SEARCH("..",$D21,1)-1)="0","",LEFT($D21,SEARCH("..",$D21,1)-1)))</f>
         <v/>
       </c>
-      <c r="K21" s="61" t="str">
+      <c r="K21" s="60" t="str">
         <f aca="false">IF(RIGHT($D21,SEARCH("..",$D21,1)-1)="n","",IF(RIGHT($D21,SEARCH("..",$D21,1)-1)="0","",RIGHT($D21,SEARCH("..",$D21,1)-1)))</f>
         <v/>
       </c>
-      <c r="L21" s="62" t="str">
+      <c r="L21" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E21,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M21" s="62" t="str">
+      <c r="M21" s="61" t="str">
         <f aca="false">IF(L21="sh:Literal",E21,"")</f>
         <v/>
       </c>
-      <c r="N21" s="62" t="str">
+      <c r="N21" s="61" t="str">
         <f aca="false">IF($L21="sh:IRI",IF($E21&lt;&gt;"",$E21,""),"")</f>
         <v/>
       </c>
-      <c r="O21" s="63" t="str">
+      <c r="O21" s="62" t="str">
         <f aca="false">IF($L21&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E21)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -3802,35 +3785,35 @@
         <v>152</v>
       </c>
       <c r="D22" s="57" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="E22" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="F22" s="59" t="s">
+      <c r="F22" s="58" t="s">
         <v>154</v>
       </c>
-      <c r="J22" s="61" t="str">
+      <c r="J22" s="60" t="str">
         <f aca="false">IF(LEFT($D22,SEARCH("..",$D22,1)-1)="n","",IF(LEFT($D22,SEARCH("..",$D22,1)-1)="0","",LEFT($D22,SEARCH("..",$D22,1)-1)))</f>
         <v/>
       </c>
-      <c r="K22" s="61" t="str">
+      <c r="K22" s="60" t="str">
         <f aca="false">IF(RIGHT($D22,SEARCH("..",$D22,1)-1)="n","",IF(RIGHT($D22,SEARCH("..",$D22,1)-1)="0","",RIGHT($D22,SEARCH("..",$D22,1)-1)))</f>
-        <v>1</v>
-      </c>
-      <c r="L22" s="62" t="str">
+        <v/>
+      </c>
+      <c r="L22" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E22,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:Literal</v>
       </c>
-      <c r="M22" s="62" t="str">
+      <c r="M22" s="61" t="str">
         <f aca="false">IF(L22="sh:Literal",E22,"")</f>
         <v>xsd:string</v>
       </c>
-      <c r="N22" s="62" t="str">
+      <c r="N22" s="61" t="str">
         <f aca="false">IF($L22="sh:IRI",IF($E22&lt;&gt;"",$E22,""),"")</f>
         <v/>
       </c>
-      <c r="O22" s="63" t="str">
+      <c r="O22" s="62" t="str">
         <f aca="false">IF($L22&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E22)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -3847,88 +3830,89 @@
         <v>155</v>
       </c>
       <c r="D23" s="57" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="E23" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="F23" s="59" t="s">
+      <c r="F23" s="58" t="s">
         <v>156</v>
       </c>
-      <c r="J23" s="61" t="str">
+      <c r="J23" s="60" t="str">
         <f aca="false">IF(LEFT($D23,SEARCH("..",$D23,1)-1)="n","",IF(LEFT($D23,SEARCH("..",$D23,1)-1)="0","",LEFT($D23,SEARCH("..",$D23,1)-1)))</f>
         <v/>
       </c>
-      <c r="K23" s="61" t="str">
+      <c r="K23" s="60" t="str">
         <f aca="false">IF(RIGHT($D23,SEARCH("..",$D23,1)-1)="n","",IF(RIGHT($D23,SEARCH("..",$D23,1)-1)="0","",RIGHT($D23,SEARCH("..",$D23,1)-1)))</f>
         <v/>
       </c>
-      <c r="L23" s="62" t="str">
+      <c r="L23" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E23,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M23" s="62" t="str">
+      <c r="M23" s="61" t="str">
         <f aca="false">IF(L23="sh:Literal",E23,"")</f>
         <v/>
       </c>
-      <c r="N23" s="62" t="str">
+      <c r="N23" s="61" t="str">
         <f aca="false">IF($L23="sh:IRI",IF($E23&lt;&gt;"",$E23,""),"")</f>
         <v>ecrm:E42_Identifier</v>
       </c>
-      <c r="O23" s="63" t="str">
+      <c r="O23" s="62" t="str">
         <f aca="false">IF($L23&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E23)-1,0)=0,"","1"))</f>
         <v/>
       </c>
     </row>
-    <row r="24" s="68" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="66" t="str">
+    <row r="24" s="66" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="65" t="str">
         <f aca="false">CONCATENATE("mus:P",ROW(A24))</f>
         <v>mus:P24</v>
       </c>
-      <c r="B24" s="67" t="s">
+      <c r="B24" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="68" t="s">
+      <c r="C24" s="66" t="s">
         <v>157</v>
       </c>
       <c r="D24" s="67" t="s">
-        <v>144</v>
-      </c>
-      <c r="E24" s="69" t="s">
+        <v>134</v>
+      </c>
+      <c r="E24" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="F24" s="59" t="s">
+      <c r="F24" s="58" t="s">
         <v>158</v>
       </c>
-      <c r="G24" s="70"/>
-      <c r="H24" s="70"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="72" t="str">
+      <c r="G24" s="69"/>
+      <c r="H24" s="69"/>
+      <c r="I24" s="70"/>
+      <c r="J24" s="71" t="str">
         <f aca="false">IF(LEFT($D24,SEARCH("..",$D24,1)-1)="n","",IF(LEFT($D24,SEARCH("..",$D24,1)-1)="0","",LEFT($D24,SEARCH("..",$D24,1)-1)))</f>
         <v/>
       </c>
-      <c r="K24" s="72" t="str">
+      <c r="K24" s="71" t="str">
         <f aca="false">IF(RIGHT($D24,SEARCH("..",$D24,1)-1)="n","",IF(RIGHT($D24,SEARCH("..",$D24,1)-1)="0","",RIGHT($D24,SEARCH("..",$D24,1)-1)))</f>
         <v/>
       </c>
-      <c r="L24" s="73" t="str">
+      <c r="L24" s="72" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E24,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M24" s="73" t="str">
+      <c r="M24" s="72" t="str">
         <f aca="false">IF(L24="sh:Literal",E24,"")</f>
         <v/>
       </c>
-      <c r="N24" s="62" t="str">
+      <c r="N24" s="61" t="str">
         <f aca="false">IF($L24="sh:IRI",IF($E24&lt;&gt;"",$E24,""),"")</f>
         <v>mus:M167_Publication_Expression_Fragment</v>
       </c>
-      <c r="O24" s="74" t="str">
+      <c r="O24" s="73" t="str">
         <f aca="false">IF($L24&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E24)-1,0)=0,"","1"))</f>
         <v/>
       </c>
-      <c r="X24" s="70"/>
-      <c r="AMJ24" s="22"/>
+      <c r="W24" s="69"/>
+      <c r="AMI24" s="22"/>
+      <c r="AMJ24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="56" t="str">
@@ -3942,35 +3926,35 @@
         <v>159</v>
       </c>
       <c r="D25" s="57" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="E25" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="F25" s="59" t="s">
+      <c r="F25" s="58" t="s">
         <v>160</v>
       </c>
-      <c r="J25" s="61" t="str">
+      <c r="J25" s="60" t="str">
         <f aca="false">IF(LEFT($D25,SEARCH("..",$D25,1)-1)="n","",IF(LEFT($D25,SEARCH("..",$D25,1)-1)="0","",LEFT($D25,SEARCH("..",$D25,1)-1)))</f>
         <v/>
       </c>
-      <c r="K25" s="61" t="str">
+      <c r="K25" s="60" t="str">
         <f aca="false">IF(RIGHT($D25,SEARCH("..",$D25,1)-1)="n","",IF(RIGHT($D25,SEARCH("..",$D25,1)-1)="0","",RIGHT($D25,SEARCH("..",$D25,1)-1)))</f>
         <v/>
       </c>
-      <c r="L25" s="62" t="str">
+      <c r="L25" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E25,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M25" s="62" t="str">
+      <c r="M25" s="61" t="str">
         <f aca="false">IF(L25="sh:Literal",E25,"")</f>
         <v/>
       </c>
-      <c r="N25" s="62" t="str">
+      <c r="N25" s="61" t="str">
         <f aca="false">IF($L25="sh:IRI",IF($E25&lt;&gt;"",$E25,""),"")</f>
         <v>mus:M6_Casting</v>
       </c>
-      <c r="O25" s="63" t="str">
+      <c r="O25" s="62" t="str">
         <f aca="false">IF($L25&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E25)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -3985,7 +3969,8 @@
       <c r="J26" s="54"/>
       <c r="K26" s="54"/>
       <c r="O26" s="53"/>
-      <c r="X26" s="55"/>
+      <c r="W26" s="55"/>
+      <c r="AMI26" s="0"/>
       <c r="AMJ26" s="0"/>
     </row>
     <row r="27" s="57" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3993,46 +3978,47 @@
         <f aca="false">CONCATENATE("mus:P",ROW(A27))</f>
         <v>mus:P27</v>
       </c>
-      <c r="B27" s="75" t="s">
+      <c r="B27" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="C27" s="58" t="s">
+      <c r="C27" s="22" t="s">
         <v>124</v>
       </c>
       <c r="D27" s="57" t="s">
         <v>125</v>
       </c>
       <c r="E27" s="24"/>
-      <c r="F27" s="59" t="s">
+      <c r="F27" s="58" t="s">
         <v>126</v>
       </c>
-      <c r="G27" s="59"/>
-      <c r="I27" s="60"/>
-      <c r="J27" s="61" t="str">
+      <c r="G27" s="58"/>
+      <c r="I27" s="59"/>
+      <c r="J27" s="60" t="str">
         <f aca="false">IF(LEFT($D27,SEARCH("..",$D27,1)-1)="n","",IF(LEFT($D27,SEARCH("..",$D27,1)-1)="0","",LEFT($D27,SEARCH("..",$D27,1)-1)))</f>
         <v/>
       </c>
-      <c r="K27" s="61" t="str">
+      <c r="K27" s="60" t="str">
         <f aca="false">IF(RIGHT($D27,SEARCH("..",$D27,1)-1)="n","",IF(RIGHT($D27,SEARCH("..",$D27,1)-1)="0","",RIGHT($D27,SEARCH("..",$D27,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="L27" s="62" t="str">
+      <c r="L27" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E27,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M27" s="62" t="str">
+      <c r="M27" s="61" t="str">
         <f aca="false">IF(L27="sh:Literal",E27,"")</f>
         <v/>
       </c>
-      <c r="N27" s="62" t="str">
+      <c r="N27" s="61" t="str">
         <f aca="false">IF($L27="sh:IRI",IF($E27&lt;&gt;"",$E27,""),"")</f>
         <v/>
       </c>
-      <c r="O27" s="63" t="str">
+      <c r="O27" s="62" t="str">
         <f aca="false">IF($L27&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E27)-1,0)=0,"","1"))</f>
         <v/>
       </c>
-      <c r="W27" s="64"/>
+      <c r="V27" s="63"/>
+      <c r="AMI27" s="0"/>
       <c r="AMJ27" s="0"/>
     </row>
     <row r="28" s="57" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4040,7 +4026,7 @@
         <f aca="false">CONCATENATE("mus:P",ROW(A28))</f>
         <v>mus:P28</v>
       </c>
-      <c r="B28" s="75" t="s">
+      <c r="B28" s="57" t="s">
         <v>73</v>
       </c>
       <c r="C28" s="57" t="s">
@@ -4049,38 +4035,39 @@
       <c r="D28" s="57" t="s">
         <v>125</v>
       </c>
-      <c r="E28" s="60"/>
-      <c r="F28" s="59" t="s">
+      <c r="E28" s="59"/>
+      <c r="F28" s="58" t="s">
         <v>128</v>
       </c>
-      <c r="G28" s="64"/>
-      <c r="H28" s="64"/>
-      <c r="I28" s="65"/>
-      <c r="J28" s="61" t="str">
+      <c r="G28" s="63"/>
+      <c r="H28" s="63"/>
+      <c r="I28" s="64"/>
+      <c r="J28" s="60" t="str">
         <f aca="false">IF(LEFT($D28,SEARCH("..",$D28,1)-1)="n","",IF(LEFT($D28,SEARCH("..",$D28,1)-1)="0","",LEFT($D28,SEARCH("..",$D28,1)-1)))</f>
         <v/>
       </c>
-      <c r="K28" s="61" t="str">
+      <c r="K28" s="60" t="str">
         <f aca="false">IF(RIGHT($D28,SEARCH("..",$D28,1)-1)="n","",IF(RIGHT($D28,SEARCH("..",$D28,1)-1)="0","",RIGHT($D28,SEARCH("..",$D28,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="L28" s="62" t="str">
+      <c r="L28" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E28,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M28" s="62" t="str">
+      <c r="M28" s="61" t="str">
         <f aca="false">IF(L28="sh:Literal",E28,"")</f>
         <v/>
       </c>
-      <c r="N28" s="62" t="str">
+      <c r="N28" s="61" t="str">
         <f aca="false">IF($L28="sh:IRI",IF($E28&lt;&gt;"",$E28,""),"")</f>
         <v/>
       </c>
-      <c r="O28" s="63" t="str">
+      <c r="O28" s="62" t="str">
         <f aca="false">IF($L28&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E28)-1,0)=0,"","1"))</f>
         <v/>
       </c>
-      <c r="W28" s="64"/>
+      <c r="V28" s="63"/>
+      <c r="AMI28" s="0"/>
       <c r="AMJ28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4088,7 +4075,7 @@
         <f aca="false">CONCATENATE("mus:P",ROW(A29))</f>
         <v>mus:P29</v>
       </c>
-      <c r="B29" s="75" t="s">
+      <c r="B29" s="57" t="s">
         <v>73</v>
       </c>
       <c r="C29" s="0" t="s">
@@ -4100,30 +4087,30 @@
       <c r="E29" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="F29" s="59" t="s">
+      <c r="F29" s="58" t="s">
         <v>130</v>
       </c>
-      <c r="J29" s="61" t="str">
+      <c r="J29" s="60" t="str">
         <f aca="false">IF(LEFT($D29,SEARCH("..",$D29,1)-1)="n","",IF(LEFT($D29,SEARCH("..",$D29,1)-1)="0","",LEFT($D29,SEARCH("..",$D29,1)-1)))</f>
         <v/>
       </c>
-      <c r="K29" s="61" t="str">
+      <c r="K29" s="60" t="str">
         <f aca="false">IF(RIGHT($D29,SEARCH("..",$D29,1)-1)="n","",IF(RIGHT($D29,SEARCH("..",$D29,1)-1)="0","",RIGHT($D29,SEARCH("..",$D29,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="L29" s="62" t="str">
+      <c r="L29" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E29,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M29" s="62" t="str">
+      <c r="M29" s="61" t="str">
         <f aca="false">IF(L29="sh:Literal",E29,"")</f>
         <v/>
       </c>
-      <c r="N29" s="62" t="str">
+      <c r="N29" s="61" t="str">
         <f aca="false">IF($L29="sh:IRI",IF($E29&lt;&gt;"",$E29,""),"")</f>
         <v>mus:M156_Title_Statement</v>
       </c>
-      <c r="O29" s="63" t="str">
+      <c r="O29" s="62" t="str">
         <f aca="false">IF($L29&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E29)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -4133,7 +4120,7 @@
         <f aca="false">CONCATENATE("mus:P",ROW(A30))</f>
         <v>mus:P30</v>
       </c>
-      <c r="B30" s="75" t="s">
+      <c r="B30" s="57" t="s">
         <v>73</v>
       </c>
       <c r="C30" s="0" t="s">
@@ -4145,30 +4132,30 @@
       <c r="E30" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="F30" s="59" t="s">
+      <c r="F30" s="58" t="s">
         <v>132</v>
       </c>
-      <c r="J30" s="61" t="str">
+      <c r="J30" s="60" t="str">
         <f aca="false">IF(LEFT($D30,SEARCH("..",$D30,1)-1)="n","",IF(LEFT($D30,SEARCH("..",$D30,1)-1)="0","",LEFT($D30,SEARCH("..",$D30,1)-1)))</f>
         <v/>
       </c>
-      <c r="K30" s="61" t="str">
+      <c r="K30" s="60" t="str">
         <f aca="false">IF(RIGHT($D30,SEARCH("..",$D30,1)-1)="n","",IF(RIGHT($D30,SEARCH("..",$D30,1)-1)="0","",RIGHT($D30,SEARCH("..",$D30,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="L30" s="62" t="str">
+      <c r="L30" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E30,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M30" s="62" t="str">
+      <c r="M30" s="61" t="str">
         <f aca="false">IF(L30="sh:Literal",E30,"")</f>
         <v/>
       </c>
-      <c r="N30" s="62" t="str">
+      <c r="N30" s="61" t="str">
         <f aca="false">IF($L30="sh:IRI",IF($E30&lt;&gt;"",$E30,""),"")</f>
         <v>mus:M157_Statement_of_Responsibility</v>
       </c>
-      <c r="O30" s="63" t="str">
+      <c r="O30" s="62" t="str">
         <f aca="false">IF($L30&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E30)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -4178,42 +4165,42 @@
         <f aca="false">CONCATENATE("mus:P",ROW(A31))</f>
         <v>mus:P31</v>
       </c>
-      <c r="B31" s="75" t="s">
+      <c r="B31" s="57" t="s">
         <v>73</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>133</v>
       </c>
       <c r="D31" s="57" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="E31" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="F31" s="59" t="s">
-        <v>134</v>
-      </c>
-      <c r="J31" s="61" t="str">
+      <c r="F31" s="58" t="s">
+        <v>135</v>
+      </c>
+      <c r="J31" s="60" t="str">
         <f aca="false">IF(LEFT($D31,SEARCH("..",$D31,1)-1)="n","",IF(LEFT($D31,SEARCH("..",$D31,1)-1)="0","",LEFT($D31,SEARCH("..",$D31,1)-1)))</f>
         <v/>
       </c>
-      <c r="K31" s="61" t="str">
+      <c r="K31" s="60" t="str">
         <f aca="false">IF(RIGHT($D31,SEARCH("..",$D31,1)-1)="n","",IF(RIGHT($D31,SEARCH("..",$D31,1)-1)="0","",RIGHT($D31,SEARCH("..",$D31,1)-1)))</f>
-        <v>1</v>
-      </c>
-      <c r="L31" s="62" t="str">
+        <v/>
+      </c>
+      <c r="L31" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E31,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M31" s="62" t="str">
+      <c r="M31" s="61" t="str">
         <f aca="false">IF(L31="sh:Literal",E31,"")</f>
         <v/>
       </c>
-      <c r="N31" s="62" t="str">
+      <c r="N31" s="61" t="str">
         <f aca="false">IF($L31="sh:IRI",IF($E31&lt;&gt;"",$E31,""),"")</f>
         <v>ecrm:E35_Title</v>
       </c>
-      <c r="O31" s="63" t="str">
+      <c r="O31" s="62" t="str">
         <f aca="false">IF($L31&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E31)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -4223,42 +4210,42 @@
         <f aca="false">CONCATENATE("mus:P",ROW(A32))</f>
         <v>mus:P32</v>
       </c>
-      <c r="B32" s="75" t="s">
+      <c r="B32" s="57" t="s">
         <v>73</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D32" s="57" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="E32" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="F32" s="59" t="s">
-        <v>136</v>
-      </c>
-      <c r="J32" s="61" t="str">
+      <c r="F32" s="58" t="s">
+        <v>137</v>
+      </c>
+      <c r="J32" s="60" t="str">
         <f aca="false">IF(LEFT($D32,SEARCH("..",$D32,1)-1)="n","",IF(LEFT($D32,SEARCH("..",$D32,1)-1)="0","",LEFT($D32,SEARCH("..",$D32,1)-1)))</f>
         <v/>
       </c>
-      <c r="K32" s="61" t="str">
+      <c r="K32" s="60" t="str">
         <f aca="false">IF(RIGHT($D32,SEARCH("..",$D32,1)-1)="n","",IF(RIGHT($D32,SEARCH("..",$D32,1)-1)="0","",RIGHT($D32,SEARCH("..",$D32,1)-1)))</f>
-        <v>1</v>
-      </c>
-      <c r="L32" s="62" t="str">
+        <v/>
+      </c>
+      <c r="L32" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E32,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M32" s="62" t="str">
+      <c r="M32" s="61" t="str">
         <f aca="false">IF(L32="sh:Literal",E32,"")</f>
         <v/>
       </c>
-      <c r="N32" s="62" t="str">
+      <c r="N32" s="61" t="str">
         <f aca="false">IF($L32="sh:IRI",IF($E32&lt;&gt;"",$E32,""),"")</f>
         <v>ecrm:E35_Title</v>
       </c>
-      <c r="O32" s="63" t="str">
+      <c r="O32" s="62" t="str">
         <f aca="false">IF($L32&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E32)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -4268,42 +4255,42 @@
         <f aca="false">CONCATENATE("mus:P",ROW(A33))</f>
         <v>mus:P33</v>
       </c>
-      <c r="B33" s="75" t="s">
+      <c r="B33" s="57" t="s">
         <v>73</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D33" s="57" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="E33" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="F33" s="59" t="s">
-        <v>138</v>
-      </c>
-      <c r="J33" s="61" t="str">
+      <c r="F33" s="58" t="s">
+        <v>139</v>
+      </c>
+      <c r="J33" s="60" t="str">
         <f aca="false">IF(LEFT($D33,SEARCH("..",$D33,1)-1)="n","",IF(LEFT($D33,SEARCH("..",$D33,1)-1)="0","",LEFT($D33,SEARCH("..",$D33,1)-1)))</f>
         <v/>
       </c>
-      <c r="K33" s="61" t="str">
+      <c r="K33" s="60" t="str">
         <f aca="false">IF(RIGHT($D33,SEARCH("..",$D33,1)-1)="n","",IF(RIGHT($D33,SEARCH("..",$D33,1)-1)="0","",RIGHT($D33,SEARCH("..",$D33,1)-1)))</f>
-        <v>1</v>
-      </c>
-      <c r="L33" s="62" t="str">
+        <v/>
+      </c>
+      <c r="L33" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E33,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M33" s="62" t="str">
+      <c r="M33" s="61" t="str">
         <f aca="false">IF(L33="sh:Literal",E33,"")</f>
         <v/>
       </c>
-      <c r="N33" s="62" t="str">
+      <c r="N33" s="61" t="str">
         <f aca="false">IF($L33="sh:IRI",IF($E33&lt;&gt;"",$E33,""),"")</f>
         <v>mus:M159_Edition_Statement</v>
       </c>
-      <c r="O33" s="63" t="str">
+      <c r="O33" s="62" t="str">
         <f aca="false">IF($L33&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E33)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -4313,11 +4300,11 @@
         <f aca="false">CONCATENATE("mus:P",ROW(A34))</f>
         <v>mus:P34</v>
       </c>
-      <c r="B34" s="75" t="s">
+      <c r="B34" s="57" t="s">
         <v>73</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D34" s="57" t="s">
         <v>125</v>
@@ -4325,30 +4312,30 @@
       <c r="E34" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="F34" s="59" t="s">
-        <v>140</v>
-      </c>
-      <c r="J34" s="61" t="str">
+      <c r="F34" s="58" t="s">
+        <v>141</v>
+      </c>
+      <c r="J34" s="60" t="str">
         <f aca="false">IF(LEFT($D34,SEARCH("..",$D34,1)-1)="n","",IF(LEFT($D34,SEARCH("..",$D34,1)-1)="0","",LEFT($D34,SEARCH("..",$D34,1)-1)))</f>
         <v/>
       </c>
-      <c r="K34" s="61" t="str">
+      <c r="K34" s="60" t="str">
         <f aca="false">IF(RIGHT($D34,SEARCH("..",$D34,1)-1)="n","",IF(RIGHT($D34,SEARCH("..",$D34,1)-1)="0","",RIGHT($D34,SEARCH("..",$D34,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="L34" s="62" t="str">
+      <c r="L34" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E34,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M34" s="62" t="str">
+      <c r="M34" s="61" t="str">
         <f aca="false">IF(L34="sh:Literal",E34,"")</f>
         <v/>
       </c>
-      <c r="N34" s="62" t="str">
+      <c r="N34" s="61" t="str">
         <f aca="false">IF($L34="sh:IRI",IF($E34&lt;&gt;"",$E34,""),"")</f>
         <v>mus:M163_Music_Format_Statement</v>
       </c>
-      <c r="O34" s="63" t="str">
+      <c r="O34" s="62" t="str">
         <f aca="false">IF($L34&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E34)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -4358,42 +4345,42 @@
         <f aca="false">CONCATENATE("mus:P",ROW(A35))</f>
         <v>mus:P35</v>
       </c>
-      <c r="B35" s="75" t="s">
+      <c r="B35" s="57" t="s">
         <v>73</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D35" s="57" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="E35" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="F35" s="59" t="s">
-        <v>142</v>
-      </c>
-      <c r="J35" s="61" t="str">
+      <c r="F35" s="58" t="s">
+        <v>143</v>
+      </c>
+      <c r="J35" s="60" t="str">
         <f aca="false">IF(LEFT($D35,SEARCH("..",$D35,1)-1)="n","",IF(LEFT($D35,SEARCH("..",$D35,1)-1)="0","",LEFT($D35,SEARCH("..",$D35,1)-1)))</f>
         <v/>
       </c>
-      <c r="K35" s="61" t="str">
+      <c r="K35" s="60" t="str">
         <f aca="false">IF(RIGHT($D35,SEARCH("..",$D35,1)-1)="n","",IF(RIGHT($D35,SEARCH("..",$D35,1)-1)="0","",RIGHT($D35,SEARCH("..",$D35,1)-1)))</f>
-        <v>1</v>
-      </c>
-      <c r="L35" s="62" t="str">
+        <v/>
+      </c>
+      <c r="L35" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E35,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M35" s="62" t="str">
+      <c r="M35" s="61" t="str">
         <f aca="false">IF(L35="sh:Literal",E35,"")</f>
         <v/>
       </c>
-      <c r="N35" s="62" t="str">
+      <c r="N35" s="61" t="str">
         <f aca="false">IF($L35="sh:IRI",IF($E35&lt;&gt;"",$E35,""),"")</f>
         <v>mus:M160_Publication_Statement</v>
       </c>
-      <c r="O35" s="63" t="str">
+      <c r="O35" s="62" t="str">
         <f aca="false">IF($L35&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E35)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -4403,39 +4390,39 @@
         <f aca="false">CONCATENATE("mus:P",ROW(A36))</f>
         <v>mus:P36</v>
       </c>
-      <c r="B36" s="75" t="s">
+      <c r="B36" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="58" t="s">
-        <v>143</v>
+      <c r="C36" s="22" t="s">
+        <v>144</v>
       </c>
       <c r="D36" s="57" t="s">
-        <v>144</v>
-      </c>
-      <c r="F36" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="F36" s="58" t="s">
         <v>145</v>
       </c>
-      <c r="J36" s="61" t="str">
+      <c r="J36" s="60" t="str">
         <f aca="false">IF(LEFT($D36,SEARCH("..",$D36,1)-1)="n","",IF(LEFT($D36,SEARCH("..",$D36,1)-1)="0","",LEFT($D36,SEARCH("..",$D36,1)-1)))</f>
         <v/>
       </c>
-      <c r="K36" s="61" t="str">
+      <c r="K36" s="60" t="str">
         <f aca="false">IF(RIGHT($D36,SEARCH("..",$D36,1)-1)="n","",IF(RIGHT($D36,SEARCH("..",$D36,1)-1)="0","",RIGHT($D36,SEARCH("..",$D36,1)-1)))</f>
         <v/>
       </c>
-      <c r="L36" s="62" t="str">
+      <c r="L36" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E36,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M36" s="62" t="str">
+      <c r="M36" s="61" t="str">
         <f aca="false">IF(L36="sh:Literal",E36,"")</f>
         <v/>
       </c>
-      <c r="N36" s="62" t="str">
+      <c r="N36" s="61" t="str">
         <f aca="false">IF($L36="sh:IRI",IF($E36&lt;&gt;"",$E36,""),"")</f>
         <v/>
       </c>
-      <c r="O36" s="63" t="str">
+      <c r="O36" s="62" t="str">
         <f aca="false">IF($L36&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E36)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -4445,39 +4432,39 @@
         <f aca="false">CONCATENATE("mus:P",ROW(A37))</f>
         <v>mus:P37</v>
       </c>
-      <c r="B37" s="75" t="s">
+      <c r="B37" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="C37" s="58" t="s">
+      <c r="C37" s="22" t="s">
         <v>146</v>
       </c>
       <c r="D37" s="57" t="s">
-        <v>144</v>
-      </c>
-      <c r="F37" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="F37" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="J37" s="61" t="str">
+      <c r="J37" s="60" t="str">
         <f aca="false">IF(LEFT($D37,SEARCH("..",$D37,1)-1)="n","",IF(LEFT($D37,SEARCH("..",$D37,1)-1)="0","",LEFT($D37,SEARCH("..",$D37,1)-1)))</f>
         <v/>
       </c>
-      <c r="K37" s="61" t="str">
+      <c r="K37" s="60" t="str">
         <f aca="false">IF(RIGHT($D37,SEARCH("..",$D37,1)-1)="n","",IF(RIGHT($D37,SEARCH("..",$D37,1)-1)="0","",RIGHT($D37,SEARCH("..",$D37,1)-1)))</f>
         <v/>
       </c>
-      <c r="L37" s="62" t="str">
+      <c r="L37" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E37,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M37" s="62" t="str">
+      <c r="M37" s="61" t="str">
         <f aca="false">IF(L37="sh:Literal",E37,"")</f>
         <v/>
       </c>
-      <c r="N37" s="62" t="str">
+      <c r="N37" s="61" t="str">
         <f aca="false">IF($L37="sh:IRI",IF($E37&lt;&gt;"",$E37,""),"")</f>
         <v/>
       </c>
-      <c r="O37" s="63" t="str">
+      <c r="O37" s="62" t="str">
         <f aca="false">IF($L37&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E37)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -4487,39 +4474,39 @@
         <f aca="false">CONCATENATE("mus:P",ROW(A38))</f>
         <v>mus:P38</v>
       </c>
-      <c r="B38" s="75" t="s">
+      <c r="B38" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="C38" s="58" t="s">
+      <c r="C38" s="22" t="s">
         <v>148</v>
       </c>
       <c r="D38" s="57" t="s">
-        <v>144</v>
-      </c>
-      <c r="F38" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="F38" s="58" t="s">
         <v>149</v>
       </c>
-      <c r="J38" s="61" t="str">
+      <c r="J38" s="60" t="str">
         <f aca="false">IF(LEFT($D38,SEARCH("..",$D38,1)-1)="n","",IF(LEFT($D38,SEARCH("..",$D38,1)-1)="0","",LEFT($D38,SEARCH("..",$D38,1)-1)))</f>
         <v/>
       </c>
-      <c r="K38" s="61" t="str">
+      <c r="K38" s="60" t="str">
         <f aca="false">IF(RIGHT($D38,SEARCH("..",$D38,1)-1)="n","",IF(RIGHT($D38,SEARCH("..",$D38,1)-1)="0","",RIGHT($D38,SEARCH("..",$D38,1)-1)))</f>
         <v/>
       </c>
-      <c r="L38" s="62" t="str">
+      <c r="L38" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E38,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M38" s="62" t="str">
+      <c r="M38" s="61" t="str">
         <f aca="false">IF(L38="sh:Literal",E38,"")</f>
         <v/>
       </c>
-      <c r="N38" s="62" t="str">
+      <c r="N38" s="61" t="str">
         <f aca="false">IF($L38="sh:IRI",IF($E38&lt;&gt;"",$E38,""),"")</f>
         <v/>
       </c>
-      <c r="O38" s="63" t="str">
+      <c r="O38" s="62" t="str">
         <f aca="false">IF($L38&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E38)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -4529,39 +4516,39 @@
         <f aca="false">CONCATENATE("mus:P",ROW(A39))</f>
         <v>mus:P39</v>
       </c>
-      <c r="B39" s="75" t="s">
+      <c r="B39" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="58" t="s">
+      <c r="C39" s="22" t="s">
         <v>150</v>
       </c>
       <c r="D39" s="57" t="s">
-        <v>144</v>
-      </c>
-      <c r="F39" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="F39" s="58" t="s">
         <v>151</v>
       </c>
-      <c r="J39" s="61" t="str">
+      <c r="J39" s="60" t="str">
         <f aca="false">IF(LEFT($D39,SEARCH("..",$D39,1)-1)="n","",IF(LEFT($D39,SEARCH("..",$D39,1)-1)="0","",LEFT($D39,SEARCH("..",$D39,1)-1)))</f>
         <v/>
       </c>
-      <c r="K39" s="61" t="str">
+      <c r="K39" s="60" t="str">
         <f aca="false">IF(RIGHT($D39,SEARCH("..",$D39,1)-1)="n","",IF(RIGHT($D39,SEARCH("..",$D39,1)-1)="0","",RIGHT($D39,SEARCH("..",$D39,1)-1)))</f>
         <v/>
       </c>
-      <c r="L39" s="62" t="str">
+      <c r="L39" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E39,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M39" s="62" t="str">
+      <c r="M39" s="61" t="str">
         <f aca="false">IF(L39="sh:Literal",E39,"")</f>
         <v/>
       </c>
-      <c r="N39" s="62" t="str">
+      <c r="N39" s="61" t="str">
         <f aca="false">IF($L39="sh:IRI",IF($E39&lt;&gt;"",$E39,""),"")</f>
         <v/>
       </c>
-      <c r="O39" s="63" t="str">
+      <c r="O39" s="62" t="str">
         <f aca="false">IF($L39&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E39)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -4571,42 +4558,42 @@
         <f aca="false">CONCATENATE("mus:P",ROW(A40))</f>
         <v>mus:P40</v>
       </c>
-      <c r="B40" s="75" t="s">
+      <c r="B40" s="57" t="s">
         <v>73</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>152</v>
       </c>
       <c r="D40" s="57" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="E40" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="F40" s="59" t="s">
+      <c r="F40" s="58" t="s">
         <v>154</v>
       </c>
-      <c r="J40" s="61" t="str">
+      <c r="J40" s="60" t="str">
         <f aca="false">IF(LEFT($D40,SEARCH("..",$D40,1)-1)="n","",IF(LEFT($D40,SEARCH("..",$D40,1)-1)="0","",LEFT($D40,SEARCH("..",$D40,1)-1)))</f>
         <v/>
       </c>
-      <c r="K40" s="61" t="str">
+      <c r="K40" s="60" t="str">
         <f aca="false">IF(RIGHT($D40,SEARCH("..",$D40,1)-1)="n","",IF(RIGHT($D40,SEARCH("..",$D40,1)-1)="0","",RIGHT($D40,SEARCH("..",$D40,1)-1)))</f>
-        <v>1</v>
-      </c>
-      <c r="L40" s="62" t="str">
+        <v/>
+      </c>
+      <c r="L40" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E40,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:Literal</v>
       </c>
-      <c r="M40" s="62" t="str">
+      <c r="M40" s="61" t="str">
         <f aca="false">IF(L40="sh:Literal",E40,"")</f>
         <v>xsd:string</v>
       </c>
-      <c r="N40" s="62" t="str">
+      <c r="N40" s="61" t="str">
         <f aca="false">IF($L40="sh:IRI",IF($E40&lt;&gt;"",$E40,""),"")</f>
         <v/>
       </c>
-      <c r="O40" s="63" t="str">
+      <c r="O40" s="62" t="str">
         <f aca="false">IF($L40&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E40)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -4616,42 +4603,42 @@
         <f aca="false">CONCATENATE("mus:P",ROW(A41))</f>
         <v>mus:P41</v>
       </c>
-      <c r="B41" s="75" t="s">
+      <c r="B41" s="57" t="s">
         <v>73</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>155</v>
       </c>
       <c r="D41" s="57" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="E41" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="F41" s="59" t="s">
+      <c r="F41" s="58" t="s">
         <v>156</v>
       </c>
-      <c r="J41" s="61" t="str">
+      <c r="J41" s="60" t="str">
         <f aca="false">IF(LEFT($D41,SEARCH("..",$D41,1)-1)="n","",IF(LEFT($D41,SEARCH("..",$D41,1)-1)="0","",LEFT($D41,SEARCH("..",$D41,1)-1)))</f>
         <v/>
       </c>
-      <c r="K41" s="61" t="str">
+      <c r="K41" s="60" t="str">
         <f aca="false">IF(RIGHT($D41,SEARCH("..",$D41,1)-1)="n","",IF(RIGHT($D41,SEARCH("..",$D41,1)-1)="0","",RIGHT($D41,SEARCH("..",$D41,1)-1)))</f>
         <v/>
       </c>
-      <c r="L41" s="62" t="str">
+      <c r="L41" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E41,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M41" s="62" t="str">
+      <c r="M41" s="61" t="str">
         <f aca="false">IF(L41="sh:Literal",E41,"")</f>
         <v/>
       </c>
-      <c r="N41" s="62" t="str">
+      <c r="N41" s="61" t="str">
         <f aca="false">IF($L41="sh:IRI",IF($E41&lt;&gt;"",$E41,""),"")</f>
         <v>ecrm:E42_Identifier</v>
       </c>
-      <c r="O41" s="63" t="str">
+      <c r="O41" s="62" t="str">
         <f aca="false">IF($L41&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E41)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -4661,49 +4648,49 @@
         <f aca="false">CONCATENATE("mus:P",ROW(A42))</f>
         <v>mus:P42</v>
       </c>
-      <c r="B42" s="75" t="s">
+      <c r="B42" s="57" t="s">
         <v>73</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>159</v>
       </c>
       <c r="D42" s="57" t="s">
-        <v>144</v>
+        <v>162</v>
       </c>
       <c r="E42" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="F42" s="59" t="s">
+      <c r="F42" s="58" t="s">
         <v>160</v>
       </c>
-      <c r="J42" s="61" t="str">
+      <c r="J42" s="60" t="str">
         <f aca="false">IF(LEFT($D42,SEARCH("..",$D42,1)-1)="n","",IF(LEFT($D42,SEARCH("..",$D42,1)-1)="0","",LEFT($D42,SEARCH("..",$D42,1)-1)))</f>
-        <v/>
-      </c>
-      <c r="K42" s="61" t="str">
+        <v>1</v>
+      </c>
+      <c r="K42" s="60" t="str">
         <f aca="false">IF(RIGHT($D42,SEARCH("..",$D42,1)-1)="n","",IF(RIGHT($D42,SEARCH("..",$D42,1)-1)="0","",RIGHT($D42,SEARCH("..",$D42,1)-1)))</f>
         <v/>
       </c>
-      <c r="L42" s="62" t="str">
+      <c r="L42" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E42,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M42" s="62" t="str">
+      <c r="M42" s="61" t="str">
         <f aca="false">IF(L42="sh:Literal",E42,"")</f>
         <v/>
       </c>
-      <c r="N42" s="62" t="str">
+      <c r="N42" s="61" t="str">
         <f aca="false">IF($L42="sh:IRI",IF($E42&lt;&gt;"",$E42,""),"")</f>
         <v>mus:M6_Casting</v>
       </c>
-      <c r="O42" s="63" t="str">
+      <c r="O42" s="62" t="str">
         <f aca="false">IF($L42&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E42)-1,0)=0,"","1"))</f>
         <v/>
       </c>
     </row>
     <row r="43" s="50" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="50" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E43" s="51"/>
       <c r="F43" s="52"/>
@@ -4711,7 +4698,8 @@
       <c r="J43" s="54"/>
       <c r="K43" s="54"/>
       <c r="O43" s="53"/>
-      <c r="X43" s="55"/>
+      <c r="W43" s="55"/>
+      <c r="AMI43" s="0"/>
       <c r="AMJ43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4719,42 +4707,42 @@
         <f aca="false">CONCATENATE("mus:P",ROW(A44))</f>
         <v>mus:P44</v>
       </c>
-      <c r="B44" s="75" t="s">
+      <c r="B44" s="57" t="s">
         <v>60</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D44" s="57" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E44" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="F44" s="59" t="s">
-        <v>165</v>
-      </c>
-      <c r="J44" s="61" t="str">
+      <c r="F44" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="J44" s="60" t="str">
         <f aca="false">IF(LEFT($D44,SEARCH("..",$D44,1)-1)="n","",IF(LEFT($D44,SEARCH("..",$D44,1)-1)="0","",LEFT($D44,SEARCH("..",$D44,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="K44" s="61" t="str">
+      <c r="K44" s="60" t="str">
         <f aca="false">IF(RIGHT($D44,SEARCH("..",$D44,1)-1)="n","",IF(RIGHT($D44,SEARCH("..",$D44,1)-1)="0","",RIGHT($D44,SEARCH("..",$D44,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="L44" s="62" t="str">
+      <c r="L44" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E44,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M44" s="62" t="str">
+      <c r="M44" s="61" t="str">
         <f aca="false">IF(L44="sh:Literal",E44,"")</f>
         <v/>
       </c>
-      <c r="N44" s="62" t="str">
+      <c r="N44" s="61" t="str">
         <f aca="false">IF($L44="sh:IRI",IF($E44&lt;&gt;"",$E44,""),"")</f>
         <v>efrbroo:F24_Publication_Expression</v>
       </c>
-      <c r="O44" s="63" t="str">
+      <c r="O44" s="62" t="str">
         <f aca="false">IF($L44&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E44)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -4764,42 +4752,42 @@
         <f aca="false">CONCATENATE("mus:P",ROW(A45))</f>
         <v>mus:P45</v>
       </c>
-      <c r="B45" s="75" t="s">
+      <c r="B45" s="57" t="s">
         <v>60</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D45" s="57" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="E45" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="F45" s="59" t="s">
-        <v>167</v>
-      </c>
-      <c r="J45" s="61" t="str">
+      <c r="F45" s="58" t="s">
+        <v>168</v>
+      </c>
+      <c r="J45" s="60" t="str">
         <f aca="false">IF(LEFT($D45,SEARCH("..",$D45,1)-1)="n","",IF(LEFT($D45,SEARCH("..",$D45,1)-1)="0","",LEFT($D45,SEARCH("..",$D45,1)-1)))</f>
         <v/>
       </c>
-      <c r="K45" s="61" t="str">
+      <c r="K45" s="60" t="str">
         <f aca="false">IF(RIGHT($D45,SEARCH("..",$D45,1)-1)="n","",IF(RIGHT($D45,SEARCH("..",$D45,1)-1)="0","",RIGHT($D45,SEARCH("..",$D45,1)-1)))</f>
         <v/>
       </c>
-      <c r="L45" s="62" t="str">
+      <c r="L45" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E45,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M45" s="62" t="str">
+      <c r="M45" s="61" t="str">
         <f aca="false">IF(L45="sh:Literal",E45,"")</f>
         <v/>
       </c>
-      <c r="N45" s="62" t="str">
+      <c r="N45" s="61" t="str">
         <f aca="false">IF($L45="sh:IRI",IF($E45&lt;&gt;"",$E45,""),"")</f>
         <v>ecrm:E7_Activity</v>
       </c>
-      <c r="O45" s="63" t="str">
+      <c r="O45" s="62" t="str">
         <f aca="false">IF($L45&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E45)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -4809,49 +4797,49 @@
         <f aca="false">CONCATENATE("mus:P",ROW(A46))</f>
         <v>mus:P46</v>
       </c>
-      <c r="B46" s="75" t="s">
+      <c r="B46" s="57" t="s">
         <v>60</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D46" s="57" t="s">
         <v>125</v>
       </c>
-      <c r="E46" s="76" t="s">
+      <c r="E46" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="F46" s="59" t="s">
-        <v>169</v>
-      </c>
-      <c r="J46" s="61" t="str">
+      <c r="F46" s="58" t="s">
+        <v>170</v>
+      </c>
+      <c r="J46" s="60" t="str">
         <f aca="false">IF(LEFT($D46,SEARCH("..",$D46,1)-1)="n","",IF(LEFT($D46,SEARCH("..",$D46,1)-1)="0","",LEFT($D46,SEARCH("..",$D46,1)-1)))</f>
         <v/>
       </c>
-      <c r="K46" s="61" t="str">
+      <c r="K46" s="60" t="str">
         <f aca="false">IF(RIGHT($D46,SEARCH("..",$D46,1)-1)="n","",IF(RIGHT($D46,SEARCH("..",$D46,1)-1)="0","",RIGHT($D46,SEARCH("..",$D46,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="L46" s="62" t="str">
+      <c r="L46" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E46,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M46" s="62" t="str">
+      <c r="M46" s="61" t="str">
         <f aca="false">IF(L46="sh:Literal",E46,"")</f>
         <v/>
       </c>
-      <c r="N46" s="62" t="str">
+      <c r="N46" s="61" t="str">
         <f aca="false">IF($L46="sh:IRI",IF($E46&lt;&gt;"",$E46,""),"")</f>
         <v>ecrm:E52_Time-Span</v>
       </c>
-      <c r="O46" s="63" t="str">
+      <c r="O46" s="62" t="str">
         <f aca="false">IF($L46&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E46)-1,0)=0,"","1"))</f>
         <v/>
       </c>
     </row>
     <row r="47" s="50" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="50" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E47" s="51"/>
       <c r="F47" s="52"/>
@@ -4859,7 +4847,8 @@
       <c r="J47" s="54"/>
       <c r="K47" s="54"/>
       <c r="O47" s="53"/>
-      <c r="X47" s="55"/>
+      <c r="W47" s="55"/>
+      <c r="AMI47" s="0"/>
       <c r="AMJ47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4871,35 +4860,35 @@
         <v>62</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D48" s="57" t="s">
-        <v>144</v>
-      </c>
-      <c r="F48" s="59" t="s">
-        <v>172</v>
-      </c>
-      <c r="J48" s="61" t="str">
+        <v>162</v>
+      </c>
+      <c r="F48" s="58" t="s">
+        <v>173</v>
+      </c>
+      <c r="J48" s="60" t="str">
         <f aca="false">IF(LEFT($D48,SEARCH("..",$D48,1)-1)="n","",IF(LEFT($D48,SEARCH("..",$D48,1)-1)="0","",LEFT($D48,SEARCH("..",$D48,1)-1)))</f>
-        <v/>
-      </c>
-      <c r="K48" s="61" t="str">
+        <v>1</v>
+      </c>
+      <c r="K48" s="60" t="str">
         <f aca="false">IF(RIGHT($D48,SEARCH("..",$D48,1)-1)="n","",IF(RIGHT($D48,SEARCH("..",$D48,1)-1)="0","",RIGHT($D48,SEARCH("..",$D48,1)-1)))</f>
         <v/>
       </c>
-      <c r="L48" s="62" t="str">
+      <c r="L48" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E48,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M48" s="62" t="str">
+      <c r="M48" s="61" t="str">
         <f aca="false">IF(L48="sh:Literal",E48,"")</f>
         <v/>
       </c>
-      <c r="N48" s="62" t="str">
+      <c r="N48" s="61" t="str">
         <f aca="false">IF($L48="sh:IRI",IF($E48&lt;&gt;"",$E48,""),"")</f>
         <v/>
       </c>
-      <c r="O48" s="63" t="str">
+      <c r="O48" s="62" t="str">
         <f aca="false">IF($L48&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E48)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -4913,42 +4902,42 @@
         <v>62</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D49" s="57" t="s">
-        <v>144</v>
-      </c>
-      <c r="F49" s="59" t="s">
-        <v>174</v>
-      </c>
-      <c r="J49" s="61" t="str">
+        <v>134</v>
+      </c>
+      <c r="F49" s="58" t="s">
+        <v>175</v>
+      </c>
+      <c r="J49" s="60" t="str">
         <f aca="false">IF(LEFT($D49,SEARCH("..",$D49,1)-1)="n","",IF(LEFT($D49,SEARCH("..",$D49,1)-1)="0","",LEFT($D49,SEARCH("..",$D49,1)-1)))</f>
         <v/>
       </c>
-      <c r="K49" s="61" t="str">
+      <c r="K49" s="60" t="str">
         <f aca="false">IF(RIGHT($D49,SEARCH("..",$D49,1)-1)="n","",IF(RIGHT($D49,SEARCH("..",$D49,1)-1)="0","",RIGHT($D49,SEARCH("..",$D49,1)-1)))</f>
         <v/>
       </c>
-      <c r="L49" s="62" t="str">
+      <c r="L49" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E49,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M49" s="62" t="str">
+      <c r="M49" s="61" t="str">
         <f aca="false">IF(L49="sh:Literal",E49,"")</f>
         <v/>
       </c>
-      <c r="N49" s="62" t="str">
+      <c r="N49" s="61" t="str">
         <f aca="false">IF($L49="sh:IRI",IF($E49&lt;&gt;"",$E49,""),"")</f>
         <v/>
       </c>
-      <c r="O49" s="63" t="str">
+      <c r="O49" s="62" t="str">
         <f aca="false">IF($L49&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E49)-1,0)=0,"","1"))</f>
         <v/>
       </c>
     </row>
     <row r="50" s="50" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="50" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E50" s="51"/>
       <c r="F50" s="52"/>
@@ -4956,7 +4945,8 @@
       <c r="J50" s="54"/>
       <c r="K50" s="54"/>
       <c r="O50" s="53"/>
-      <c r="X50" s="55"/>
+      <c r="W50" s="55"/>
+      <c r="AMI50" s="0"/>
       <c r="AMJ50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4968,41 +4958,41 @@
         <v>63</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D51" s="57" t="s">
         <v>125</v>
       </c>
       <c r="E51" s="57" t="s">
-        <v>177</v>
-      </c>
-      <c r="F51" s="59" t="s">
         <v>178</v>
       </c>
-      <c r="H51" s="77" t="s">
+      <c r="F51" s="58" t="s">
         <v>179</v>
       </c>
-      <c r="J51" s="61" t="str">
-        <f aca="false">IF(LEFT($D51,SEARCH("..",$D51,1)-1)="n","",IF(LEFT($D51,SEARCH("..",$D51,1)-1)="0","",LEFT($D51,SEARCH("..",$D51,1)-1)))</f>
-        <v/>
-      </c>
-      <c r="K51" s="61" t="str">
+      <c r="H51" s="74" t="s">
+        <v>180</v>
+      </c>
+      <c r="J51" s="60" t="str">
         <f aca="false">IF(RIGHT($D51,SEARCH("..",$D51,1)-1)="n","",IF(RIGHT($D51,SEARCH("..",$D51,1)-1)="0","",RIGHT($D51,SEARCH("..",$D51,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="L51" s="62" t="str">
+      <c r="K51" s="60" t="str">
+        <f aca="false">IF(RIGHT($D51,SEARCH("..",$D51,1)-1)="n","",IF(RIGHT($D51,SEARCH("..",$D51,1)-1)="0","",RIGHT($D51,SEARCH("..",$D51,1)-1)))</f>
+        <v>1</v>
+      </c>
+      <c r="L51" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E51,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:Literal</v>
       </c>
-      <c r="M51" s="62" t="str">
+      <c r="M51" s="61" t="str">
         <f aca="false">IF(L51="sh:Literal",E51,"")</f>
         <v>xsd:integer</v>
       </c>
-      <c r="N51" s="62" t="str">
+      <c r="N51" s="61" t="str">
         <f aca="false">IF($L51="sh:IRI",IF($E51&lt;&gt;"",$E51,""),"")</f>
         <v/>
       </c>
-      <c r="O51" s="63" t="str">
+      <c r="O51" s="62" t="str">
         <f aca="false">IF($L51&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E51)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -5016,39 +5006,39 @@
         <v>63</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D52" s="57" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="E52" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="F52" s="78" t="s">
+      <c r="F52" s="75" t="s">
         <v>182</v>
       </c>
-      <c r="H52" s="77"/>
-      <c r="J52" s="61" t="str">
+      <c r="H52" s="74"/>
+      <c r="J52" s="60" t="str">
         <f aca="false">IF(LEFT($D52,SEARCH("..",$D52,1)-1)="n","",IF(LEFT($D52,SEARCH("..",$D52,1)-1)="0","",LEFT($D52,SEARCH("..",$D52,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="K52" s="61" t="str">
+      <c r="K52" s="60" t="str">
         <f aca="false">IF(RIGHT($D52,SEARCH("..",$D52,1)-1)="n","",IF(RIGHT($D52,SEARCH("..",$D52,1)-1)="0","",RIGHT($D52,SEARCH("..",$D52,1)-1)))</f>
         <v/>
       </c>
-      <c r="L52" s="62" t="str">
+      <c r="L52" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E52,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M52" s="62" t="str">
+      <c r="M52" s="61" t="str">
         <f aca="false">IF(L52="sh:Literal",E52,"")</f>
         <v/>
       </c>
-      <c r="N52" s="62" t="str">
+      <c r="N52" s="61" t="str">
         <f aca="false">IF($L52="sh:IRI",IF($E52&lt;&gt;"",$E52,""),"")</f>
         <v>mus:M23_Casting_Detail</v>
       </c>
-      <c r="O52" s="63" t="str">
+      <c r="O52" s="62" t="str">
         <f aca="false">IF($L52&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E52)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -5063,7 +5053,8 @@
       <c r="J53" s="54"/>
       <c r="K53" s="54"/>
       <c r="O53" s="53"/>
-      <c r="X53" s="55"/>
+      <c r="W53" s="55"/>
+      <c r="AMI53" s="0"/>
       <c r="AMJ53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5078,35 +5069,35 @@
         <v>184</v>
       </c>
       <c r="D54" s="57" t="s">
-        <v>164</v>
-      </c>
-      <c r="F54" s="59" t="s">
+        <v>165</v>
+      </c>
+      <c r="F54" s="58" t="s">
         <v>185</v>
       </c>
-      <c r="H54" s="59" t="s">
+      <c r="H54" s="58" t="s">
         <v>186</v>
       </c>
-      <c r="J54" s="61" t="str">
+      <c r="J54" s="60" t="str">
         <f aca="false">IF(LEFT($D54,SEARCH("..",$D54,1)-1)="n","",IF(LEFT($D54,SEARCH("..",$D54,1)-1)="0","",LEFT($D54,SEARCH("..",$D54,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="K54" s="61" t="str">
+      <c r="K54" s="60" t="str">
         <f aca="false">IF(RIGHT($D54,SEARCH("..",$D54,1)-1)="n","",IF(RIGHT($D54,SEARCH("..",$D54,1)-1)="0","",RIGHT($D54,SEARCH("..",$D54,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="L54" s="62" t="str">
+      <c r="L54" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E54,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M54" s="62" t="str">
+      <c r="M54" s="61" t="str">
         <f aca="false">IF(L54="sh:Literal",E54,"")</f>
         <v/>
       </c>
-      <c r="N54" s="62" t="str">
+      <c r="N54" s="61" t="str">
         <f aca="false">IF($L54="sh:IRI",IF($E54&lt;&gt;"",$E54,""),"")</f>
         <v/>
       </c>
-      <c r="O54" s="63" t="str">
+      <c r="O54" s="62" t="str">
         <f aca="false">IF($L54&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E54)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -5125,31 +5116,31 @@
       <c r="D55" s="57" t="s">
         <v>125</v>
       </c>
-      <c r="E55" s="79"/>
-      <c r="F55" s="59" t="s">
+      <c r="E55" s="76"/>
+      <c r="F55" s="58" t="s">
         <v>188</v>
       </c>
-      <c r="J55" s="61" t="str">
+      <c r="J55" s="60" t="str">
         <f aca="false">IF(LEFT($D55,SEARCH("..",$D55,1)-1)="n","",IF(LEFT($D55,SEARCH("..",$D55,1)-1)="0","",LEFT($D55,SEARCH("..",$D55,1)-1)))</f>
         <v/>
       </c>
-      <c r="K55" s="61" t="str">
+      <c r="K55" s="60" t="str">
         <f aca="false">IF(RIGHT($D55,SEARCH("..",$D55,1)-1)="n","",IF(RIGHT($D55,SEARCH("..",$D55,1)-1)="0","",RIGHT($D55,SEARCH("..",$D55,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="L55" s="62" t="str">
+      <c r="L55" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E55,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M55" s="62" t="str">
+      <c r="M55" s="61" t="str">
         <f aca="false">IF(L55="sh:Literal",E55,"")</f>
         <v/>
       </c>
-      <c r="N55" s="62" t="str">
+      <c r="N55" s="61" t="str">
         <f aca="false">IF($L55="sh:IRI",IF($E55&lt;&gt;"",$E55,""),"")</f>
         <v/>
       </c>
-      <c r="O55" s="63" t="str">
+      <c r="O55" s="62" t="str">
         <f aca="false">IF($L55&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E55)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -5168,30 +5159,30 @@
       <c r="D56" s="57" t="s">
         <v>125</v>
       </c>
-      <c r="F56" s="59" t="s">
+      <c r="F56" s="58" t="s">
         <v>190</v>
       </c>
-      <c r="J56" s="61" t="str">
+      <c r="J56" s="60" t="str">
         <f aca="false">IF(LEFT($D56,SEARCH("..",$D56,1)-1)="n","",IF(LEFT($D56,SEARCH("..",$D56,1)-1)="0","",LEFT($D56,SEARCH("..",$D56,1)-1)))</f>
         <v/>
       </c>
-      <c r="K56" s="61" t="str">
+      <c r="K56" s="60" t="str">
         <f aca="false">IF(RIGHT($D56,SEARCH("..",$D56,1)-1)="n","",IF(RIGHT($D56,SEARCH("..",$D56,1)-1)="0","",RIGHT($D56,SEARCH("..",$D56,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="L56" s="62" t="str">
+      <c r="L56" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E56,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M56" s="62" t="str">
+      <c r="M56" s="61" t="str">
         <f aca="false">IF(L56="sh:Literal",E56,"")</f>
         <v/>
       </c>
-      <c r="N56" s="62" t="str">
+      <c r="N56" s="61" t="str">
         <f aca="false">IF($L56="sh:IRI",IF($E56&lt;&gt;"",$E56,""),"")</f>
         <v/>
       </c>
-      <c r="O56" s="63" t="str">
+      <c r="O56" s="62" t="str">
         <f aca="false">IF($L56&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E56)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -5208,38 +5199,38 @@
         <v>191</v>
       </c>
       <c r="D57" s="57" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E57" s="57" t="s">
-        <v>177</v>
-      </c>
-      <c r="F57" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="F57" s="58" t="s">
         <v>192</v>
       </c>
-      <c r="H57" s="78" t="s">
+      <c r="H57" s="75" t="s">
         <v>193</v>
       </c>
-      <c r="J57" s="61" t="str">
+      <c r="J57" s="60" t="str">
         <f aca="false">IF(LEFT($D57,SEARCH("..",$D57,1)-1)="n","",IF(LEFT($D57,SEARCH("..",$D57,1)-1)="0","",LEFT($D57,SEARCH("..",$D57,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="K57" s="61" t="str">
+      <c r="K57" s="60" t="str">
         <f aca="false">IF(RIGHT($D57,SEARCH("..",$D57,1)-1)="n","",IF(RIGHT($D57,SEARCH("..",$D57,1)-1)="0","",RIGHT($D57,SEARCH("..",$D57,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="L57" s="62" t="str">
+      <c r="L57" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E57,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:Literal</v>
       </c>
-      <c r="M57" s="62" t="str">
+      <c r="M57" s="61" t="str">
         <f aca="false">IF(L57="sh:Literal",E57,"")</f>
         <v>xsd:integer</v>
       </c>
-      <c r="N57" s="62" t="str">
+      <c r="N57" s="61" t="str">
         <f aca="false">IF($L57="sh:IRI",IF($E57&lt;&gt;"",$E57,""),"")</f>
         <v/>
       </c>
-      <c r="O57" s="63" t="str">
+      <c r="O57" s="62" t="str">
         <f aca="false">IF($L57&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E57)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -5256,36 +5247,36 @@
         <v>152</v>
       </c>
       <c r="D58" s="57" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="E58" s="57" t="s">
         <v>153</v>
       </c>
-      <c r="F58" s="59" t="s">
+      <c r="F58" s="58" t="s">
         <v>154</v>
       </c>
-      <c r="H58" s="78"/>
-      <c r="J58" s="61" t="str">
+      <c r="H58" s="75"/>
+      <c r="J58" s="60" t="str">
         <f aca="false">IF(LEFT($D58,SEARCH("..",$D58,1)-1)="n","",IF(LEFT($D58,SEARCH("..",$D58,1)-1)="0","",LEFT($D58,SEARCH("..",$D58,1)-1)))</f>
         <v/>
       </c>
-      <c r="K58" s="61" t="str">
+      <c r="K58" s="60" t="str">
         <f aca="false">IF(RIGHT($D58,SEARCH("..",$D58,1)-1)="n","",IF(RIGHT($D58,SEARCH("..",$D58,1)-1)="0","",RIGHT($D58,SEARCH("..",$D58,1)-1)))</f>
-        <v>1</v>
-      </c>
-      <c r="L58" s="62" t="str">
+        <v/>
+      </c>
+      <c r="L58" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E58,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:Literal</v>
       </c>
-      <c r="M58" s="62" t="str">
+      <c r="M58" s="61" t="str">
         <f aca="false">IF(L58="sh:Literal",E58,"")</f>
         <v>xsd:string</v>
       </c>
-      <c r="N58" s="62" t="str">
+      <c r="N58" s="61" t="str">
         <f aca="false">IF($L58="sh:IRI",IF($E58&lt;&gt;"",$E58,""),"")</f>
         <v/>
       </c>
-      <c r="O58" s="63" t="str">
+      <c r="O58" s="62" t="str">
         <f aca="false">IF($L58&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E58)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -5304,31 +5295,31 @@
       <c r="D59" s="57" t="s">
         <v>125</v>
       </c>
-      <c r="F59" s="59" t="s">
+      <c r="F59" s="58" t="s">
         <v>195</v>
       </c>
-      <c r="H59" s="78"/>
-      <c r="J59" s="61" t="str">
+      <c r="H59" s="75"/>
+      <c r="J59" s="60" t="str">
         <f aca="false">IF(LEFT($D59,SEARCH("..",$D59,1)-1)="n","",IF(LEFT($D59,SEARCH("..",$D59,1)-1)="0","",LEFT($D59,SEARCH("..",$D59,1)-1)))</f>
         <v/>
       </c>
-      <c r="K59" s="61" t="str">
+      <c r="K59" s="60" t="str">
         <f aca="false">IF(RIGHT($D59,SEARCH("..",$D59,1)-1)="n","",IF(RIGHT($D59,SEARCH("..",$D59,1)-1)="0","",RIGHT($D59,SEARCH("..",$D59,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="L59" s="62" t="str">
+      <c r="L59" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E59,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M59" s="62" t="str">
+      <c r="M59" s="61" t="str">
         <f aca="false">IF(L59="sh:Literal",E59,"")</f>
         <v/>
       </c>
-      <c r="N59" s="62" t="str">
+      <c r="N59" s="61" t="str">
         <f aca="false">IF($L59="sh:IRI",IF($E59&lt;&gt;"",$E59,""),"")</f>
         <v/>
       </c>
-      <c r="O59" s="63" t="str">
+      <c r="O59" s="62" t="str">
         <f aca="false">IF($L59&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E59)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -5343,10 +5334,11 @@
       <c r="J60" s="54"/>
       <c r="K60" s="54"/>
       <c r="O60" s="53"/>
-      <c r="X60" s="55"/>
+      <c r="W60" s="55"/>
+      <c r="AMI60" s="0"/>
       <c r="AMJ60" s="0"/>
     </row>
-    <row r="61" s="80" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" s="77" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="56" t="str">
         <f aca="false">CONCATENATE("mus:P",ROW(A61))</f>
         <v>mus:P61</v>
@@ -5358,40 +5350,41 @@
         <v>21</v>
       </c>
       <c r="D61" s="57" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E61" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="F61" s="59" t="s">
+      <c r="F61" s="58" t="s">
         <v>197</v>
       </c>
-      <c r="I61" s="81"/>
-      <c r="J61" s="61" t="str">
+      <c r="I61" s="78"/>
+      <c r="J61" s="60" t="str">
         <f aca="false">IF(LEFT($D61,SEARCH("..",$D61,1)-1)="n","",IF(LEFT($D61,SEARCH("..",$D61,1)-1)="0","",LEFT($D61,SEARCH("..",$D61,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="K61" s="61" t="str">
+      <c r="K61" s="60" t="str">
         <f aca="false">IF(RIGHT($D61,SEARCH("..",$D61,1)-1)="n","",IF(RIGHT($D61,SEARCH("..",$D61,1)-1)="0","",RIGHT($D61,SEARCH("..",$D61,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="L61" s="62" t="str">
+      <c r="L61" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E61,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:Literal</v>
       </c>
-      <c r="M61" s="82" t="str">
+      <c r="M61" s="79" t="str">
         <f aca="false">IF(L61="sh:Literal",E61,"")</f>
         <v>xsd:string</v>
       </c>
-      <c r="N61" s="62" t="str">
+      <c r="N61" s="61" t="str">
         <f aca="false">IF($L61="sh:IRI",IF($E61&lt;&gt;"",$E61,""),"")</f>
         <v/>
       </c>
-      <c r="O61" s="82" t="str">
+      <c r="O61" s="79" t="str">
         <f aca="false">IF($L61&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E61)-1,0)=0,"","1"))</f>
         <v/>
       </c>
-      <c r="X61" s="83"/>
+      <c r="W61" s="80"/>
+      <c r="AMI61" s="0"/>
       <c r="AMJ61" s="0"/>
     </row>
     <row r="62" s="50" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5404,7 +5397,8 @@
       <c r="J62" s="54"/>
       <c r="K62" s="54"/>
       <c r="O62" s="53"/>
-      <c r="X62" s="55"/>
+      <c r="W62" s="55"/>
+      <c r="AMI62" s="0"/>
       <c r="AMJ62" s="0"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5419,35 +5413,35 @@
         <v>21</v>
       </c>
       <c r="D63" s="57" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E63" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="F63" s="59" t="s">
+      <c r="F63" s="58" t="s">
         <v>197</v>
       </c>
-      <c r="J63" s="61" t="str">
+      <c r="J63" s="60" t="str">
         <f aca="false">IF(LEFT($D63,SEARCH("..",$D63,1)-1)="n","",IF(LEFT($D63,SEARCH("..",$D63,1)-1)="0","",LEFT($D63,SEARCH("..",$D63,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="K63" s="61" t="str">
+      <c r="K63" s="60" t="str">
         <f aca="false">IF(RIGHT($D63,SEARCH("..",$D63,1)-1)="n","",IF(RIGHT($D63,SEARCH("..",$D63,1)-1)="0","",RIGHT($D63,SEARCH("..",$D63,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="L63" s="62" t="str">
+      <c r="L63" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E63,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:Literal</v>
       </c>
-      <c r="M63" s="82" t="str">
+      <c r="M63" s="79" t="str">
         <f aca="false">IF(L63="sh:Literal",E63,"")</f>
         <v>xsd:string</v>
       </c>
-      <c r="N63" s="62" t="str">
+      <c r="N63" s="61" t="str">
         <f aca="false">IF($L63="sh:IRI",IF($E63&lt;&gt;"",$E63,""),"")</f>
         <v/>
       </c>
-      <c r="O63" s="82" t="str">
+      <c r="O63" s="79" t="str">
         <f aca="false">IF($L63&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E63)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -5462,7 +5456,8 @@
       <c r="J64" s="54"/>
       <c r="K64" s="54"/>
       <c r="O64" s="53"/>
-      <c r="X64" s="55"/>
+      <c r="W64" s="55"/>
+      <c r="AMI64" s="0"/>
       <c r="AMJ64" s="0"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5477,35 +5472,35 @@
         <v>21</v>
       </c>
       <c r="D65" s="57" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E65" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="F65" s="59" t="s">
+      <c r="F65" s="58" t="s">
         <v>197</v>
       </c>
-      <c r="J65" s="61" t="str">
+      <c r="J65" s="60" t="str">
         <f aca="false">IF(LEFT($D65,SEARCH("..",$D65,1)-1)="n","",IF(LEFT($D65,SEARCH("..",$D65,1)-1)="0","",LEFT($D65,SEARCH("..",$D65,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="K65" s="61" t="str">
+      <c r="K65" s="60" t="str">
         <f aca="false">IF(RIGHT($D65,SEARCH("..",$D65,1)-1)="n","",IF(RIGHT($D65,SEARCH("..",$D65,1)-1)="0","",RIGHT($D65,SEARCH("..",$D65,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="L65" s="62" t="str">
+      <c r="L65" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E65,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:Literal</v>
       </c>
-      <c r="M65" s="82" t="str">
+      <c r="M65" s="79" t="str">
         <f aca="false">IF(L65="sh:Literal",E65,"")</f>
         <v>xsd:string</v>
       </c>
-      <c r="N65" s="62" t="str">
+      <c r="N65" s="61" t="str">
         <f aca="false">IF($L65="sh:IRI",IF($E65&lt;&gt;"",$E65,""),"")</f>
         <v/>
       </c>
-      <c r="O65" s="82" t="str">
+      <c r="O65" s="79" t="str">
         <f aca="false">IF($L65&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E65)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -5520,10 +5515,11 @@
       <c r="J66" s="54"/>
       <c r="K66" s="54"/>
       <c r="O66" s="53"/>
-      <c r="X66" s="55"/>
+      <c r="W66" s="55"/>
+      <c r="AMI66" s="0"/>
       <c r="AMJ66" s="0"/>
     </row>
-    <row r="67" s="80" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" s="77" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="56" t="str">
         <f aca="false">CONCATENATE("mus:P",ROW(A67))</f>
         <v>mus:P67</v>
@@ -5535,40 +5531,41 @@
         <v>21</v>
       </c>
       <c r="D67" s="57" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E67" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="F67" s="59" t="s">
+      <c r="F67" s="58" t="s">
         <v>197</v>
       </c>
-      <c r="I67" s="81"/>
-      <c r="J67" s="61" t="str">
+      <c r="I67" s="78"/>
+      <c r="J67" s="60" t="str">
         <f aca="false">IF(LEFT($D67,SEARCH("..",$D67,1)-1)="n","",IF(LEFT($D67,SEARCH("..",$D67,1)-1)="0","",LEFT($D67,SEARCH("..",$D67,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="K67" s="61" t="str">
+      <c r="K67" s="60" t="str">
         <f aca="false">IF(RIGHT($D67,SEARCH("..",$D67,1)-1)="n","",IF(RIGHT($D67,SEARCH("..",$D67,1)-1)="0","",RIGHT($D67,SEARCH("..",$D67,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="L67" s="62" t="str">
+      <c r="L67" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E67,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:Literal</v>
       </c>
-      <c r="M67" s="82" t="str">
+      <c r="M67" s="79" t="str">
         <f aca="false">IF(L67="sh:Literal",E67,"")</f>
         <v>xsd:string</v>
       </c>
-      <c r="N67" s="62" t="str">
+      <c r="N67" s="61" t="str">
         <f aca="false">IF($L67="sh:IRI",IF($E67&lt;&gt;"",$E67,""),"")</f>
         <v/>
       </c>
-      <c r="O67" s="82" t="str">
+      <c r="O67" s="79" t="str">
         <f aca="false">IF($L67&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E67)-1,0)=0,"","1"))</f>
         <v/>
       </c>
-      <c r="X67" s="83"/>
+      <c r="W67" s="80"/>
+      <c r="AMI67" s="0"/>
       <c r="AMJ67" s="0"/>
     </row>
     <row r="68" s="50" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5581,10 +5578,11 @@
       <c r="J68" s="54"/>
       <c r="K68" s="54"/>
       <c r="O68" s="53"/>
-      <c r="X68" s="55"/>
+      <c r="W68" s="55"/>
+      <c r="AMI68" s="0"/>
       <c r="AMJ68" s="0"/>
     </row>
-    <row r="69" s="80" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" s="77" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="56" t="str">
         <f aca="false">CONCATENATE("mus:P",ROW(A69))</f>
         <v>mus:P69</v>
@@ -5596,40 +5594,41 @@
         <v>21</v>
       </c>
       <c r="D69" s="57" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E69" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="F69" s="59" t="s">
+      <c r="F69" s="58" t="s">
         <v>197</v>
       </c>
-      <c r="I69" s="81"/>
-      <c r="J69" s="61" t="str">
+      <c r="I69" s="78"/>
+      <c r="J69" s="60" t="str">
         <f aca="false">IF(LEFT($D69,SEARCH("..",$D69,1)-1)="n","",IF(LEFT($D69,SEARCH("..",$D69,1)-1)="0","",LEFT($D69,SEARCH("..",$D69,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="K69" s="61" t="str">
+      <c r="K69" s="60" t="str">
         <f aca="false">IF(RIGHT($D69,SEARCH("..",$D69,1)-1)="n","",IF(RIGHT($D69,SEARCH("..",$D69,1)-1)="0","",RIGHT($D69,SEARCH("..",$D69,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="L69" s="62" t="str">
+      <c r="L69" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E69,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:Literal</v>
       </c>
-      <c r="M69" s="82" t="str">
+      <c r="M69" s="79" t="str">
         <f aca="false">IF(L69="sh:Literal",E69,"")</f>
         <v>xsd:string</v>
       </c>
-      <c r="N69" s="62" t="str">
+      <c r="N69" s="61" t="str">
         <f aca="false">IF($L69="sh:IRI",IF($E69&lt;&gt;"",$E69,""),"")</f>
         <v/>
       </c>
-      <c r="O69" s="82" t="str">
+      <c r="O69" s="79" t="str">
         <f aca="false">IF($L69&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E69)-1,0)=0,"","1"))</f>
         <v/>
       </c>
-      <c r="X69" s="83"/>
+      <c r="W69" s="80"/>
+      <c r="AMI69" s="0"/>
       <c r="AMJ69" s="0"/>
     </row>
     <row r="70" s="50" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5642,7 +5641,8 @@
       <c r="J70" s="54"/>
       <c r="K70" s="54"/>
       <c r="O70" s="53"/>
-      <c r="X70" s="55"/>
+      <c r="W70" s="55"/>
+      <c r="AMI70" s="0"/>
       <c r="AMJ70" s="0"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5657,35 +5657,35 @@
         <v>21</v>
       </c>
       <c r="D71" s="57" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E71" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="F71" s="59" t="s">
+      <c r="F71" s="58" t="s">
         <v>197</v>
       </c>
-      <c r="J71" s="61" t="str">
+      <c r="J71" s="60" t="str">
         <f aca="false">IF(LEFT($D71,SEARCH("..",$D71,1)-1)="n","",IF(LEFT($D71,SEARCH("..",$D71,1)-1)="0","",LEFT($D71,SEARCH("..",$D71,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="K71" s="61" t="str">
+      <c r="K71" s="60" t="str">
         <f aca="false">IF(RIGHT($D71,SEARCH("..",$D71,1)-1)="n","",IF(RIGHT($D71,SEARCH("..",$D71,1)-1)="0","",RIGHT($D71,SEARCH("..",$D71,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="L71" s="62" t="str">
+      <c r="L71" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E71,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:Literal</v>
       </c>
-      <c r="M71" s="82" t="str">
+      <c r="M71" s="79" t="str">
         <f aca="false">IF(L71="sh:Literal",E71,"")</f>
         <v>xsd:string</v>
       </c>
-      <c r="N71" s="62" t="str">
+      <c r="N71" s="61" t="str">
         <f aca="false">IF($L71="sh:IRI",IF($E71&lt;&gt;"",$E71,""),"")</f>
         <v/>
       </c>
-      <c r="O71" s="82" t="str">
+      <c r="O71" s="79" t="str">
         <f aca="false">IF($L71&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E71)-1,0)=0,"","1"))</f>
         <v/>
       </c>
@@ -5700,10 +5700,11 @@
       <c r="J72" s="54"/>
       <c r="K72" s="54"/>
       <c r="O72" s="53"/>
-      <c r="X72" s="55"/>
+      <c r="W72" s="55"/>
+      <c r="AMI72" s="0"/>
       <c r="AMJ72" s="0"/>
     </row>
-    <row r="73" s="80" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" s="77" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="56" t="str">
         <f aca="false">CONCATENATE("mus:P",ROW(A73))</f>
         <v>mus:P73</v>
@@ -5715,43 +5716,44 @@
         <v>21</v>
       </c>
       <c r="D73" s="57" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E73" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="F73" s="59" t="s">
+      <c r="F73" s="58" t="s">
         <v>156</v>
       </c>
-      <c r="I73" s="81"/>
-      <c r="J73" s="61" t="str">
+      <c r="I73" s="78"/>
+      <c r="J73" s="60" t="str">
         <f aca="false">IF(LEFT($D73,SEARCH("..",$D73,1)-1)="n","",IF(LEFT($D73,SEARCH("..",$D73,1)-1)="0","",LEFT($D73,SEARCH("..",$D73,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="K73" s="61" t="str">
+      <c r="K73" s="60" t="str">
         <f aca="false">IF(RIGHT($D73,SEARCH("..",$D73,1)-1)="n","",IF(RIGHT($D73,SEARCH("..",$D73,1)-1)="0","",RIGHT($D73,SEARCH("..",$D73,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="L73" s="62" t="str">
+      <c r="L73" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E73,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:Literal</v>
       </c>
-      <c r="M73" s="82" t="str">
+      <c r="M73" s="79" t="str">
         <f aca="false">IF(L73="sh:Literal",E73,"")</f>
         <v>xsd:string</v>
       </c>
-      <c r="N73" s="62" t="str">
+      <c r="N73" s="61" t="str">
         <f aca="false">IF($L73="sh:IRI",IF($E73&lt;&gt;"",$E73,""),"")</f>
         <v/>
       </c>
-      <c r="O73" s="82" t="str">
+      <c r="O73" s="79" t="str">
         <f aca="false">IF($L73&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E73)-1,0)=0,"","1"))</f>
         <v/>
       </c>
-      <c r="X73" s="83"/>
+      <c r="W73" s="80"/>
+      <c r="AMI73" s="0"/>
       <c r="AMJ73" s="0"/>
     </row>
-    <row r="74" s="80" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" s="77" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="56" t="str">
         <f aca="false">CONCATENATE("mus:P",ROW(A74))</f>
         <v>mus:P74</v>
@@ -5763,38 +5765,39 @@
         <v>204</v>
       </c>
       <c r="D74" s="57" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E74" s="0"/>
-      <c r="F74" s="59" t="s">
+      <c r="F74" s="58" t="s">
         <v>205</v>
       </c>
-      <c r="I74" s="81"/>
-      <c r="J74" s="61" t="str">
+      <c r="I74" s="78"/>
+      <c r="J74" s="60" t="str">
         <f aca="false">IF(LEFT($D74,SEARCH("..",$D74,1)-1)="n","",IF(LEFT($D74,SEARCH("..",$D74,1)-1)="0","",LEFT($D74,SEARCH("..",$D74,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="K74" s="61" t="str">
+      <c r="K74" s="60" t="str">
         <f aca="false">IF(RIGHT($D74,SEARCH("..",$D74,1)-1)="n","",IF(RIGHT($D74,SEARCH("..",$D74,1)-1)="0","",RIGHT($D74,SEARCH("..",$D74,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="L74" s="62" t="str">
+      <c r="L74" s="61" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E74,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:IRI</v>
       </c>
-      <c r="M74" s="62" t="str">
+      <c r="M74" s="61" t="str">
         <f aca="false">IF(L74="sh:Literal",E74,"")</f>
         <v/>
       </c>
-      <c r="N74" s="62" t="str">
+      <c r="N74" s="61" t="str">
         <f aca="false">IF($L74="sh:IRI",IF($E74&lt;&gt;"",$E74,""),"")</f>
         <v/>
       </c>
-      <c r="O74" s="63" t="str">
+      <c r="O74" s="62" t="str">
         <f aca="false">IF($L74&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E74)-1,0)=0,"","1"))</f>
         <v/>
       </c>
-      <c r="X74" s="83"/>
+      <c r="W74" s="80"/>
+      <c r="AMI74" s="0"/>
       <c r="AMJ74" s="0"/>
     </row>
     <row r="75" s="50" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5807,57 +5810,59 @@
       <c r="J75" s="54"/>
       <c r="K75" s="54"/>
       <c r="O75" s="53"/>
-      <c r="X75" s="55"/>
+      <c r="W75" s="55"/>
+      <c r="AMI75" s="0"/>
       <c r="AMJ75" s="0"/>
     </row>
-    <row r="76" s="68" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="66" t="str">
+    <row r="76" s="66" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="65" t="str">
         <f aca="false">CONCATENATE("mus:P",ROW(A76))</f>
         <v>mus:P76</v>
       </c>
-      <c r="B76" s="69" t="s">
+      <c r="B76" s="68" t="s">
         <v>72</v>
       </c>
-      <c r="C76" s="68" t="s">
+      <c r="C76" s="66" t="s">
         <v>207</v>
       </c>
       <c r="D76" s="57" t="s">
-        <v>164</v>
-      </c>
-      <c r="E76" s="69" t="s">
+        <v>165</v>
+      </c>
+      <c r="E76" s="68" t="s">
         <v>208</v>
       </c>
-      <c r="F76" s="59" t="s">
-        <v>169</v>
-      </c>
-      <c r="G76" s="70"/>
-      <c r="H76" s="70"/>
-      <c r="I76" s="71"/>
-      <c r="J76" s="61" t="str">
+      <c r="F76" s="58" t="s">
+        <v>170</v>
+      </c>
+      <c r="G76" s="69"/>
+      <c r="H76" s="69"/>
+      <c r="I76" s="70"/>
+      <c r="J76" s="60" t="str">
         <f aca="false">IF(LEFT($D76,SEARCH("..",$D76,1)-1)="n","",IF(LEFT($D76,SEARCH("..",$D76,1)-1)="0","",LEFT($D76,SEARCH("..",$D76,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="K76" s="61" t="str">
+      <c r="K76" s="60" t="str">
         <f aca="false">IF(RIGHT($D76,SEARCH("..",$D76,1)-1)="n","",IF(RIGHT($D76,SEARCH("..",$D76,1)-1)="0","",RIGHT($D76,SEARCH("..",$D76,1)-1)))</f>
         <v>1</v>
       </c>
-      <c r="L76" s="73" t="str">
+      <c r="L76" s="72" t="str">
         <f aca="false">IF(IFERROR(VLOOKUP($E76,Catalogue!$A$2:$A$40,1,0),0) &lt;&gt; 0,"sh:Literal","sh:IRI")</f>
         <v>sh:Literal</v>
       </c>
-      <c r="M76" s="84" t="str">
+      <c r="M76" s="81" t="str">
         <f aca="false">IF(L76="sh:Literal",E76,"")</f>
         <v>xsd:gYear</v>
       </c>
-      <c r="N76" s="62" t="str">
+      <c r="N76" s="61" t="str">
         <f aca="false">IF($L76="sh:IRI",IF($E76&lt;&gt;"",$E76,""),"")</f>
         <v/>
       </c>
-      <c r="O76" s="84" t="str">
+      <c r="O76" s="81" t="str">
         <f aca="false">IF($L76&lt;&gt;"sh:IRI","",IF(IFERROR(SEARCH(",",$E76)-1,0)=0,"","1"))</f>
         <v/>
       </c>
-      <c r="X76" s="70"/>
+      <c r="W76" s="69"/>
+      <c r="AMI76" s="0"/>
       <c r="AMJ76" s="0"/>
     </row>
   </sheetData>
@@ -5887,25 +5892,25 @@
   <dimension ref="A1:E148"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="1" sqref="D35 A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6953125" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.32"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="82" t="s">
         <v>209</v>
       </c>
-      <c r="E1" s="85" t="s">
+      <c r="E1" s="82" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="83" t="s">
         <v>211</v>
       </c>
       <c r="E2" s="0" t="s">
@@ -5913,7 +5918,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="86" t="s">
+      <c r="A3" s="83" t="s">
         <v>213</v>
       </c>
       <c r="E3" s="0" t="s">
@@ -6034,7 +6039,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>243</v>

</xml_diff>